<commit_message>
Fin de journée 08/05/2019
Création du fichier de documentation + avancée.
Développement de la page de connexion + script deconnexion
Début de la vue de la page Avis coté client
</commit_message>
<xml_diff>
--- a/TPI/docs/Analyse/BJ_Planification.xlsx
+++ b/TPI/docs/Analyse/BJ_Planification.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="78">
   <si>
     <t>Temps nécessaire</t>
   </si>
@@ -253,6 +253,9 @@
   <si>
     <t>Afficher les demandes des clients avec leur statut (ouverte / en cours / traitée / refusée)</t>
   </si>
+  <si>
+    <t xml:space="preserve">Connexion et déconnexion du réparateur à l'application </t>
+  </si>
 </sst>
 </file>
 
@@ -434,7 +437,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -539,11 +542,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="406">
+  <dxfs count="389">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -573,13 +585,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="4" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
@@ -608,6 +613,81 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="6" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
@@ -1962,198 +2042,6 @@
         <strike val="0"/>
         <color auto="1"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="3" tint="0.79998168889431442"/>
@@ -3929,7 +3817,7 @@
   <dimension ref="A1:N59"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4152,7 +4040,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="45" t="s">
-        <v>48</v>
+        <v>77</v>
       </c>
       <c r="B9" s="34">
         <v>8.3333333333333329E-2</v>
@@ -4906,7 +4794,7 @@
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" s="55" t="s">
+      <c r="A40" s="56" t="s">
         <v>65</v>
       </c>
       <c r="B40" s="34"/>
@@ -4927,7 +4815,7 @@
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A41" s="49" t="s">
+      <c r="A41" s="52" t="s">
         <v>46</v>
       </c>
       <c r="B41" s="34">
@@ -4952,7 +4840,7 @@
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A42" s="49" t="s">
+      <c r="A42" s="52" t="s">
         <v>66</v>
       </c>
       <c r="B42" s="34">
@@ -4979,7 +4867,7 @@
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" s="47" t="s">
+      <c r="A43" s="54" t="s">
         <v>67</v>
       </c>
       <c r="B43" s="34">
@@ -5004,7 +4892,7 @@
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A44" s="46" t="s">
+      <c r="A44" s="53" t="s">
         <v>68</v>
       </c>
       <c r="B44" s="34">
@@ -5029,7 +4917,7 @@
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" s="49" t="s">
+      <c r="A45" s="52" t="s">
         <v>69</v>
       </c>
       <c r="B45" s="34">
@@ -5054,7 +4942,7 @@
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A46" s="45" t="s">
+      <c r="A46" s="57" t="s">
         <v>70</v>
       </c>
       <c r="B46" s="34">
@@ -5079,7 +4967,7 @@
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A47" s="46" t="s">
+      <c r="A47" s="53" t="s">
         <v>43</v>
       </c>
       <c r="B47" s="34">
@@ -5104,7 +4992,7 @@
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A48" s="48" t="s">
+      <c r="A48" s="58" t="s">
         <v>71</v>
       </c>
       <c r="B48" s="34"/>
@@ -5125,7 +5013,7 @@
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A49" s="49" t="s">
+      <c r="A49" s="52" t="s">
         <v>46</v>
       </c>
       <c r="B49" s="34">
@@ -5150,7 +5038,7 @@
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A50" s="45" t="s">
+      <c r="A50" s="57" t="s">
         <v>72</v>
       </c>
       <c r="B50" s="34">
@@ -5175,7 +5063,7 @@
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A51" s="45" t="s">
+      <c r="A51" s="57" t="s">
         <v>43</v>
       </c>
       <c r="B51" s="34">
@@ -5426,806 +5314,806 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:M2 E3:E5 G3:G5 I3:I5 L3:L5 C52 E52:I52 L52 C55:C56 E55:E56 G55:G56 L55:L56 C57:L57">
-    <cfRule type="cellIs" dxfId="405" priority="229" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="388" priority="229" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:M2 D4:M5 C52:M52 C55:M57">
-    <cfRule type="cellIs" dxfId="404" priority="228" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="387" priority="228" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D52 G52 J52:K52">
-    <cfRule type="cellIs" dxfId="403" priority="224" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="386" priority="224" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:M5 C52:M52 C55:M57">
-    <cfRule type="cellIs" dxfId="402" priority="221" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="401" priority="222" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="400" priority="223" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="385" priority="221" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="384" priority="222" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="383" priority="223" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2 N55:N57">
-    <cfRule type="cellIs" dxfId="399" priority="214" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="382" priority="214" operator="greaterThan">
       <formula>$B2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="398" priority="220" operator="equal">
+    <cfRule type="cellIs" dxfId="381" priority="220" operator="equal">
       <formula>$B2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B58">
-    <cfRule type="cellIs" dxfId="397" priority="216" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="380" priority="216" operator="greaterThan">
       <formula>3.66666666666667</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="396" priority="218" operator="equal">
+    <cfRule type="cellIs" dxfId="379" priority="218" operator="equal">
       <formula>3.66666666666667</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C58:M58">
-    <cfRule type="cellIs" dxfId="395" priority="215" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="378" priority="215" operator="greaterThan">
       <formula>0.333333333333333</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="394" priority="217" operator="equal">
+    <cfRule type="cellIs" dxfId="377" priority="217" operator="equal">
       <formula>0.333333333333333</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N52 N3:N5">
-    <cfRule type="cellIs" dxfId="393" priority="212" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="376" priority="212" operator="greaterThan">
       <formula>$B3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="392" priority="213" operator="equal">
+    <cfRule type="cellIs" dxfId="375" priority="213" operator="equal">
       <formula>$B3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18 E18:I18 L18">
-    <cfRule type="cellIs" dxfId="391" priority="124" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="374" priority="124" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18:M18">
-    <cfRule type="cellIs" dxfId="390" priority="123" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="373" priority="123" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17:M17">
-    <cfRule type="cellIs" dxfId="389" priority="127" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="388" priority="128" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="387" priority="129" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="372" priority="127" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="371" priority="128" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="370" priority="129" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N18">
-    <cfRule type="cellIs" dxfId="386" priority="125" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="369" priority="125" operator="greaterThan">
       <formula>$B18</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="385" priority="126" operator="equal">
+    <cfRule type="cellIs" dxfId="368" priority="126" operator="equal">
       <formula>$B18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11 E11 G11 I11 L11">
-    <cfRule type="cellIs" dxfId="384" priority="183" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="367" priority="183" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11:M11">
-    <cfRule type="cellIs" dxfId="383" priority="182" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="366" priority="182" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:C10 E6:E10 G6:G10 I6:I10 L6:L10">
-    <cfRule type="cellIs" dxfId="382" priority="190" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="365" priority="190" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:M10">
-    <cfRule type="cellIs" dxfId="381" priority="189" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="364" priority="189" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:M10">
-    <cfRule type="cellIs" dxfId="380" priority="186" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="379" priority="187" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="378" priority="188" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="363" priority="186" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="362" priority="187" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="361" priority="188" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N6:N10">
-    <cfRule type="cellIs" dxfId="377" priority="184" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="360" priority="184" operator="greaterThan">
       <formula>$B6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="376" priority="185" operator="equal">
+    <cfRule type="cellIs" dxfId="359" priority="185" operator="equal">
       <formula>$B6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L11 I11 G11 E11 C11">
-    <cfRule type="cellIs" dxfId="375" priority="181" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="358" priority="181" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11:M11">
-    <cfRule type="cellIs" dxfId="374" priority="180" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="357" priority="180" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11:M11">
-    <cfRule type="cellIs" dxfId="373" priority="177" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="372" priority="178" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="371" priority="179" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="356" priority="177" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="355" priority="178" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="354" priority="179" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N11">
-    <cfRule type="cellIs" dxfId="370" priority="175" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="353" priority="175" operator="greaterThan">
       <formula>$B11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="369" priority="176" operator="equal">
+    <cfRule type="cellIs" dxfId="352" priority="176" operator="equal">
       <formula>$B11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N12">
-    <cfRule type="cellIs" dxfId="368" priority="173" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="351" priority="173" operator="greaterThan">
       <formula>$B12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="367" priority="174" operator="equal">
+    <cfRule type="cellIs" dxfId="350" priority="174" operator="equal">
       <formula>$B12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12 E12:I12 L12">
-    <cfRule type="cellIs" dxfId="366" priority="172" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="349" priority="172" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12:M12">
-    <cfRule type="cellIs" dxfId="365" priority="171" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="348" priority="171" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12 G12 J12:K12">
-    <cfRule type="cellIs" dxfId="364" priority="170" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="347" priority="170" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12:M12">
-    <cfRule type="cellIs" dxfId="363" priority="167" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="362" priority="168" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="361" priority="169" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="346" priority="167" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="345" priority="168" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="344" priority="169" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N13">
-    <cfRule type="cellIs" dxfId="360" priority="165" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="343" priority="165" operator="greaterThan">
       <formula>$B13</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="359" priority="166" operator="equal">
+    <cfRule type="cellIs" dxfId="342" priority="166" operator="equal">
       <formula>$B13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13 E13:I13 L13">
-    <cfRule type="cellIs" dxfId="358" priority="164" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="341" priority="164" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13:M13">
-    <cfRule type="cellIs" dxfId="357" priority="163" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="340" priority="163" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13 G13 J13:K13">
-    <cfRule type="cellIs" dxfId="356" priority="162" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="339" priority="162" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13:M13">
-    <cfRule type="cellIs" dxfId="355" priority="159" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="354" priority="160" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="353" priority="161" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="338" priority="159" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="337" priority="160" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="336" priority="161" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N14">
-    <cfRule type="cellIs" dxfId="352" priority="157" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="335" priority="157" operator="greaterThan">
       <formula>$B14</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="351" priority="158" operator="equal">
+    <cfRule type="cellIs" dxfId="334" priority="158" operator="equal">
       <formula>$B14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14 E14:I14 L14">
-    <cfRule type="cellIs" dxfId="350" priority="156" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="333" priority="156" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:M14">
-    <cfRule type="cellIs" dxfId="349" priority="155" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="332" priority="155" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14 G14 J14:K14">
-    <cfRule type="cellIs" dxfId="348" priority="154" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="331" priority="154" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:M14">
-    <cfRule type="cellIs" dxfId="347" priority="151" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="346" priority="152" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="345" priority="153" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="330" priority="151" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="329" priority="152" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="328" priority="153" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N15">
-    <cfRule type="cellIs" dxfId="344" priority="149" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="327" priority="149" operator="greaterThan">
       <formula>$B15</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="343" priority="150" operator="equal">
+    <cfRule type="cellIs" dxfId="326" priority="150" operator="equal">
       <formula>$B15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15 E15:I15 L15">
-    <cfRule type="cellIs" dxfId="342" priority="148" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="325" priority="148" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:M15">
-    <cfRule type="cellIs" dxfId="341" priority="147" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="324" priority="147" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15 G15 J15:K15">
-    <cfRule type="cellIs" dxfId="340" priority="146" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="323" priority="146" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:M15">
-    <cfRule type="cellIs" dxfId="339" priority="143" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="338" priority="144" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="337" priority="145" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="322" priority="143" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="321" priority="144" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="320" priority="145" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16:M16">
-    <cfRule type="cellIs" dxfId="336" priority="135" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="335" priority="136" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="334" priority="137" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="319" priority="135" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="318" priority="136" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="317" priority="137" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N16">
-    <cfRule type="cellIs" dxfId="333" priority="141" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="316" priority="141" operator="greaterThan">
       <formula>$B16</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="332" priority="142" operator="equal">
+    <cfRule type="cellIs" dxfId="315" priority="142" operator="equal">
       <formula>$B16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16 E16:I16 L16">
-    <cfRule type="cellIs" dxfId="331" priority="140" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="314" priority="140" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16:M16">
-    <cfRule type="cellIs" dxfId="330" priority="139" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="313" priority="139" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16 G16 J16:K16">
-    <cfRule type="cellIs" dxfId="329" priority="138" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="312" priority="138" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N17">
-    <cfRule type="cellIs" dxfId="328" priority="133" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="311" priority="133" operator="greaterThan">
       <formula>$B17</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="327" priority="134" operator="equal">
+    <cfRule type="cellIs" dxfId="310" priority="134" operator="equal">
       <formula>$B17</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17 E17:I17 L17">
-    <cfRule type="cellIs" dxfId="326" priority="132" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="309" priority="132" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17:M17">
-    <cfRule type="cellIs" dxfId="325" priority="131" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="308" priority="131" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D17 G17 J17:K17">
-    <cfRule type="cellIs" dxfId="324" priority="130" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="307" priority="130" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18:M18">
-    <cfRule type="cellIs" dxfId="323" priority="119" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="322" priority="120" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="321" priority="121" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="306" priority="119" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="305" priority="120" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="304" priority="121" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18 G18 J18:K18">
-    <cfRule type="cellIs" dxfId="320" priority="122" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="303" priority="122" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19:M19">
-    <cfRule type="cellIs" dxfId="319" priority="111" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="318" priority="112" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="317" priority="113" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="302" priority="111" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="301" priority="112" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="300" priority="113" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N19">
-    <cfRule type="cellIs" dxfId="316" priority="117" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="299" priority="117" operator="greaterThan">
       <formula>$B19</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="315" priority="118" operator="equal">
+    <cfRule type="cellIs" dxfId="298" priority="118" operator="equal">
       <formula>$B19</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19 E19:I19 L19">
-    <cfRule type="cellIs" dxfId="314" priority="116" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="297" priority="116" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19:M19">
-    <cfRule type="cellIs" dxfId="313" priority="115" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="296" priority="115" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D19 G19 J19:K19">
-    <cfRule type="cellIs" dxfId="312" priority="114" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="295" priority="114" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20:M20">
-    <cfRule type="cellIs" dxfId="311" priority="103" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="310" priority="104" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="309" priority="105" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="294" priority="103" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="293" priority="104" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="292" priority="105" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N20">
-    <cfRule type="cellIs" dxfId="308" priority="109" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="291" priority="109" operator="greaterThan">
       <formula>$B20</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="307" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="290" priority="110" operator="equal">
       <formula>$B20</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20 E20:I20 L20">
-    <cfRule type="cellIs" dxfId="306" priority="108" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="289" priority="108" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20:M20">
-    <cfRule type="cellIs" dxfId="305" priority="107" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="288" priority="107" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D20 G20 J20:K20">
-    <cfRule type="cellIs" dxfId="304" priority="106" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="287" priority="106" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:M21">
-    <cfRule type="cellIs" dxfId="303" priority="95" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="302" priority="96" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="301" priority="97" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="286" priority="95" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="285" priority="96" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="284" priority="97" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N21">
-    <cfRule type="cellIs" dxfId="300" priority="101" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="283" priority="101" operator="greaterThan">
       <formula>$B21</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="299" priority="102" operator="equal">
+    <cfRule type="cellIs" dxfId="282" priority="102" operator="equal">
       <formula>$B21</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21 E21:I21 L21">
-    <cfRule type="cellIs" dxfId="298" priority="100" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="281" priority="100" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:M21">
-    <cfRule type="cellIs" dxfId="297" priority="99" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="280" priority="99" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D21 G21 J21:K21">
-    <cfRule type="cellIs" dxfId="296" priority="98" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="279" priority="98" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C25 E22:E25 G22:G25 I22:I25 L22:L25">
-    <cfRule type="cellIs" dxfId="295" priority="94" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="278" priority="94" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:M25">
-    <cfRule type="cellIs" dxfId="294" priority="93" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="277" priority="93" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:M25">
-    <cfRule type="cellIs" dxfId="293" priority="90" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="292" priority="91" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="291" priority="92" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="276" priority="90" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="275" priority="91" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="274" priority="92" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N22:N25">
-    <cfRule type="cellIs" dxfId="290" priority="88" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="273" priority="88" operator="greaterThan">
       <formula>$B22</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="289" priority="89" operator="equal">
+    <cfRule type="cellIs" dxfId="272" priority="89" operator="equal">
       <formula>$B22</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26 E26:I26 L26">
-    <cfRule type="cellIs" dxfId="288" priority="87" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="271" priority="87" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:M26">
-    <cfRule type="cellIs" dxfId="287" priority="86" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="270" priority="86" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D26 G26 J26:K26">
-    <cfRule type="cellIs" dxfId="286" priority="85" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="269" priority="85" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:M26">
-    <cfRule type="cellIs" dxfId="285" priority="82" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="284" priority="83" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="283" priority="84" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="268" priority="82" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="267" priority="83" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="266" priority="84" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N26">
-    <cfRule type="cellIs" dxfId="282" priority="80" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="265" priority="80" operator="greaterThan">
       <formula>$B26</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="281" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="264" priority="81" operator="equal">
       <formula>$B26</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27 E27:I27 L27">
-    <cfRule type="cellIs" dxfId="280" priority="79" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="263" priority="79" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27:M27">
-    <cfRule type="cellIs" dxfId="279" priority="78" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="262" priority="78" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27 G27 J27:K27">
-    <cfRule type="cellIs" dxfId="278" priority="77" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="261" priority="77" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27:M27">
-    <cfRule type="cellIs" dxfId="277" priority="74" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="276" priority="75" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="275" priority="76" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="260" priority="74" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="259" priority="75" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="258" priority="76" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N27">
-    <cfRule type="cellIs" dxfId="274" priority="72" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="257" priority="72" operator="greaterThan">
       <formula>$B27</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="273" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="256" priority="73" operator="equal">
       <formula>$B27</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:C39 E28:E39 G28:G39 I28:I39 L28:L39">
-    <cfRule type="cellIs" dxfId="272" priority="71" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="255" priority="71" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:M39 C28:M33">
-    <cfRule type="cellIs" dxfId="271" priority="70" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="254" priority="70" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:M39">
-    <cfRule type="cellIs" dxfId="270" priority="67" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="269" priority="68" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="268" priority="69" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="253" priority="67" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="252" priority="68" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="251" priority="69" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N39 N28:N30">
-    <cfRule type="cellIs" dxfId="267" priority="65" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="250" priority="65" operator="greaterThan">
       <formula>$B28</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="266" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="249" priority="66" operator="equal">
       <formula>$B28</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N31:N38">
-    <cfRule type="cellIs" dxfId="265" priority="63" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="248" priority="63" operator="greaterThan">
       <formula>$B31</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="264" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="247" priority="64" operator="equal">
       <formula>$B31</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40:C47 E40:E47 G40:G47 I40:I47 L40:L47">
-    <cfRule type="cellIs" dxfId="263" priority="55" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="246" priority="55" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40:M47">
-    <cfRule type="cellIs" dxfId="262" priority="54" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="245" priority="54" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40:M47">
-    <cfRule type="cellIs" dxfId="261" priority="51" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="260" priority="52" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="259" priority="53" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="244" priority="51" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="243" priority="52" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="242" priority="53" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N43:N47">
-    <cfRule type="cellIs" dxfId="258" priority="49" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="241" priority="49" operator="greaterThan">
       <formula>$B43</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="257" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="240" priority="50" operator="equal">
       <formula>$B43</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N40:N42">
-    <cfRule type="cellIs" dxfId="256" priority="47" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="239" priority="47" operator="greaterThan">
       <formula>$B40</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="255" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="238" priority="48" operator="equal">
       <formula>$B40</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C51 E49:E51 G49:G51 I49:I51 L49:L51">
-    <cfRule type="cellIs" dxfId="254" priority="46" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="237" priority="46" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:M51">
-    <cfRule type="cellIs" dxfId="253" priority="45" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="236" priority="45" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:M51">
-    <cfRule type="cellIs" dxfId="252" priority="42" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="251" priority="43" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="250" priority="44" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="235" priority="42" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="234" priority="43" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="233" priority="44" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N49:N51">
-    <cfRule type="cellIs" dxfId="249" priority="40" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="232" priority="40" operator="greaterThan">
       <formula>$B49</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="248" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="231" priority="41" operator="equal">
       <formula>$B49</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48 E48:I48 L48">
-    <cfRule type="cellIs" dxfId="247" priority="39" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="230" priority="39" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:M48">
-    <cfRule type="cellIs" dxfId="246" priority="38" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="229" priority="38" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D48 G48 J48:K48">
-    <cfRule type="cellIs" dxfId="245" priority="37" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="228" priority="37" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:M48">
-    <cfRule type="cellIs" dxfId="244" priority="34" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="243" priority="35" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="242" priority="36" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="227" priority="34" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="226" priority="35" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="225" priority="36" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N48">
-    <cfRule type="cellIs" dxfId="241" priority="32" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="224" priority="32" operator="greaterThan">
       <formula>$B48</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="240" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="223" priority="33" operator="equal">
       <formula>$B48</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I55:I56">
-    <cfRule type="cellIs" dxfId="239" priority="31" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="222" priority="31" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L55 I55 G55 E55 C55">
-    <cfRule type="cellIs" dxfId="238" priority="23" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="221" priority="23" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:M55">
-    <cfRule type="cellIs" dxfId="237" priority="22" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="220" priority="22" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54:M54">
-    <cfRule type="cellIs" dxfId="236" priority="6" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="235" priority="7" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="234" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="219" priority="6" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="218" priority="7" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="217" priority="8" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N53">
-    <cfRule type="cellIs" dxfId="233" priority="20" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="216" priority="20" operator="greaterThan">
       <formula>$B53</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="232" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="215" priority="21" operator="equal">
       <formula>$B53</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C53 E53:I53 L53">
-    <cfRule type="cellIs" dxfId="231" priority="19" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="214" priority="19" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C53:M53">
-    <cfRule type="cellIs" dxfId="230" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="213" priority="18" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D53 G53 J53:K53">
-    <cfRule type="cellIs" dxfId="229" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="212" priority="17" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C53:M53">
-    <cfRule type="cellIs" dxfId="228" priority="14" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="227" priority="15" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="226" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="211" priority="14" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="210" priority="15" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="209" priority="16" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N54">
-    <cfRule type="cellIs" dxfId="225" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="208" priority="12" operator="greaterThan">
       <formula>$B54</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="224" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="207" priority="13" operator="equal">
       <formula>$B54</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54 E54:I54 L54">
-    <cfRule type="cellIs" dxfId="223" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="206" priority="11" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54:M54">
-    <cfRule type="cellIs" dxfId="222" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="205" priority="10" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D54 G54 J54:K54">
-    <cfRule type="cellIs" dxfId="221" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="204" priority="9" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C5">
-    <cfRule type="cellIs" dxfId="220" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="203" priority="5" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2 C4:C5">
-    <cfRule type="cellIs" dxfId="219" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="202" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C5">
-    <cfRule type="cellIs" dxfId="218" priority="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="217" priority="2" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="216" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="201" priority="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="200" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="199" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6239,7 +6127,7 @@
   <dimension ref="A1:N59"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6374,7 +6262,9 @@
       <c r="C5" s="4">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="D5" s="13"/>
+      <c r="D5" s="13">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="E5" s="4"/>
       <c r="F5" s="13"/>
       <c r="G5" s="4"/>
@@ -6386,7 +6276,7 @@
       <c r="M5" s="15"/>
       <c r="N5" s="3">
         <f t="shared" si="0"/>
-        <v>4.1666666666666664E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -6418,7 +6308,9 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="C7" s="4"/>
-      <c r="D7" s="13"/>
+      <c r="D7" s="13">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="E7" s="4"/>
       <c r="F7" s="13"/>
       <c r="G7" s="4"/>
@@ -6430,7 +6322,7 @@
       <c r="M7" s="15"/>
       <c r="N7" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -6441,7 +6333,9 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="C8" s="4"/>
-      <c r="D8" s="13"/>
+      <c r="D8" s="13">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="E8" s="4"/>
       <c r="F8" s="13"/>
       <c r="G8" s="4"/>
@@ -6453,7 +6347,7 @@
       <c r="M8" s="15"/>
       <c r="N8" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -6464,7 +6358,9 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="C9" s="4"/>
-      <c r="D9" s="13"/>
+      <c r="D9" s="13">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="E9" s="4"/>
       <c r="F9" s="13"/>
       <c r="G9" s="4"/>
@@ -6476,7 +6372,7 @@
       <c r="M9" s="15"/>
       <c r="N9" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -6487,7 +6383,9 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="C10" s="4"/>
-      <c r="D10" s="13"/>
+      <c r="D10" s="13">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="E10" s="4"/>
       <c r="F10" s="13"/>
       <c r="G10" s="4"/>
@@ -6499,7 +6397,7 @@
       <c r="M10" s="15"/>
       <c r="N10" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -6531,7 +6429,9 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
+      <c r="D12" s="4">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
@@ -6543,7 +6443,7 @@
       <c r="M12" s="15"/>
       <c r="N12" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -7455,7 +7355,9 @@
       <c r="C53" s="4">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="D53" s="4"/>
+      <c r="D53" s="4">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="E53" s="4"/>
       <c r="F53" s="4"/>
       <c r="G53" s="4"/>
@@ -7467,7 +7369,7 @@
       <c r="M53" s="15"/>
       <c r="N53" s="3">
         <f t="shared" ref="N53:N54" si="2">SUM(C53:M53)</f>
-        <v>4.1666666666666664E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
@@ -7520,7 +7422,9 @@
       <c r="C56" s="4">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="D56" s="13"/>
+      <c r="D56" s="13">
+        <v>0.125</v>
+      </c>
       <c r="E56" s="13"/>
       <c r="F56" s="13"/>
       <c r="G56" s="13"/>
@@ -7532,7 +7436,7 @@
       <c r="M56" s="15"/>
       <c r="N56" s="3">
         <f>SUM(C56:M56)</f>
-        <v>8.3333333333333329E-2</v>
+        <v>0.20833333333333331</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
@@ -7570,7 +7474,7 @@
       </c>
       <c r="D58" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.33333333333333337</v>
       </c>
       <c r="E58" s="3">
         <f t="shared" si="3"/>
@@ -7613,815 +7517,815 @@
       <c r="A59" s="42"/>
       <c r="M59" s="3">
         <f>SUM(C58:M58)</f>
-        <v>0.33333333333333331</v>
+        <v>0.66666666666666674</v>
       </c>
       <c r="N59" s="3">
         <f>SUM(N2:N57)</f>
-        <v>0.33333333333333331</v>
+        <v>0.66666666666666652</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:M2 E3:E5 G3:G5 I3:I5 L3:L5 C52 E52:I52 L52 C55:C56 E55:E56 G55:G56 L55:L56 C57:L57">
-    <cfRule type="cellIs" dxfId="189" priority="190" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="198" priority="190" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:M2 D4:M5 C52:M52 C55:M57">
-    <cfRule type="cellIs" dxfId="188" priority="189" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="197" priority="189" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D52 G52 J52:K52">
-    <cfRule type="cellIs" dxfId="187" priority="188" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="196" priority="188" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:M5 C52:M52 C55:M57">
-    <cfRule type="cellIs" dxfId="186" priority="185" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="185" priority="186" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="184" priority="187" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="195" priority="185" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="194" priority="186" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="193" priority="187" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2 N55:N57">
-    <cfRule type="cellIs" dxfId="183" priority="179" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="192" priority="179" operator="greaterThan">
       <formula>$B2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="182" priority="184" operator="equal">
+    <cfRule type="cellIs" dxfId="191" priority="184" operator="equal">
       <formula>$B2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B58">
-    <cfRule type="cellIs" dxfId="181" priority="181" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="190" priority="181" operator="greaterThan">
       <formula>3.66666666666667</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="180" priority="183" operator="equal">
+    <cfRule type="cellIs" dxfId="189" priority="183" operator="equal">
       <formula>3.66666666666667</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C58:M58">
-    <cfRule type="cellIs" dxfId="179" priority="180" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="188" priority="180" operator="greaterThan">
       <formula>0.333333333333333</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="178" priority="182" operator="equal">
+    <cfRule type="cellIs" dxfId="187" priority="182" operator="equal">
       <formula>0.333333333333333</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N52 N3:N5">
-    <cfRule type="cellIs" dxfId="177" priority="177" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="186" priority="177" operator="greaterThan">
       <formula>$B3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="176" priority="178" operator="equal">
+    <cfRule type="cellIs" dxfId="185" priority="178" operator="equal">
       <formula>$B3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18 E18:I18 L18">
-    <cfRule type="cellIs" dxfId="175" priority="110" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="184" priority="110" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18:M18">
-    <cfRule type="cellIs" dxfId="174" priority="109" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="183" priority="109" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17:M17">
-    <cfRule type="cellIs" dxfId="173" priority="113" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="172" priority="114" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="171" priority="115" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="182" priority="113" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="181" priority="114" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="180" priority="115" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N18">
-    <cfRule type="cellIs" dxfId="170" priority="111" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="179" priority="111" operator="greaterThan">
       <formula>$B18</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="169" priority="112" operator="equal">
+    <cfRule type="cellIs" dxfId="178" priority="112" operator="equal">
       <formula>$B18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11 E11 G11 I11 L11">
-    <cfRule type="cellIs" dxfId="168" priority="169" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="177" priority="169" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11:M11">
-    <cfRule type="cellIs" dxfId="167" priority="168" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="176" priority="168" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:C10 E6:E10 G6:G10 I6:I10 L6:L10">
-    <cfRule type="cellIs" dxfId="166" priority="176" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="175" priority="176" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:M10">
-    <cfRule type="cellIs" dxfId="165" priority="175" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="174" priority="175" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:M10">
-    <cfRule type="cellIs" dxfId="164" priority="172" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="163" priority="173" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="162" priority="174" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="173" priority="172" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="172" priority="173" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="171" priority="174" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N6:N10">
-    <cfRule type="cellIs" dxfId="161" priority="170" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="170" priority="170" operator="greaterThan">
       <formula>$B6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="160" priority="171" operator="equal">
+    <cfRule type="cellIs" dxfId="169" priority="171" operator="equal">
       <formula>$B6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L11 I11 G11 E11 C11">
-    <cfRule type="cellIs" dxfId="159" priority="167" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="168" priority="167" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11:M11">
-    <cfRule type="cellIs" dxfId="158" priority="166" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="167" priority="166" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11:M11">
-    <cfRule type="cellIs" dxfId="157" priority="163" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="156" priority="164" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="155" priority="165" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="166" priority="163" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="165" priority="164" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="164" priority="165" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N11">
-    <cfRule type="cellIs" dxfId="154" priority="161" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="163" priority="161" operator="greaterThan">
       <formula>$B11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="153" priority="162" operator="equal">
+    <cfRule type="cellIs" dxfId="162" priority="162" operator="equal">
       <formula>$B11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N12">
-    <cfRule type="cellIs" dxfId="152" priority="159" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="161" priority="159" operator="greaterThan">
       <formula>$B12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="151" priority="160" operator="equal">
+    <cfRule type="cellIs" dxfId="160" priority="160" operator="equal">
       <formula>$B12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12 E12:I12 L12">
-    <cfRule type="cellIs" dxfId="150" priority="158" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="159" priority="158" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12:M12">
-    <cfRule type="cellIs" dxfId="149" priority="157" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="158" priority="157" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12 G12 J12:K12">
-    <cfRule type="cellIs" dxfId="148" priority="156" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="157" priority="156" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12:M12">
-    <cfRule type="cellIs" dxfId="147" priority="153" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="146" priority="154" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="145" priority="155" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="156" priority="153" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="155" priority="154" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="154" priority="155" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N13">
-    <cfRule type="cellIs" dxfId="144" priority="151" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="153" priority="151" operator="greaterThan">
       <formula>$B13</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="143" priority="152" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="152" operator="equal">
       <formula>$B13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13 E13:I13 L13">
-    <cfRule type="cellIs" dxfId="142" priority="150" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="151" priority="150" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13:M13">
-    <cfRule type="cellIs" dxfId="141" priority="149" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="150" priority="149" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13 G13 J13:K13">
-    <cfRule type="cellIs" dxfId="140" priority="148" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="149" priority="148" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13:M13">
-    <cfRule type="cellIs" dxfId="139" priority="145" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="138" priority="146" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="137" priority="147" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="148" priority="145" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="147" priority="146" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="146" priority="147" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N14">
-    <cfRule type="cellIs" dxfId="136" priority="143" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="145" priority="143" operator="greaterThan">
       <formula>$B14</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="135" priority="144" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="144" operator="equal">
       <formula>$B14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14 E14:I14 L14">
-    <cfRule type="cellIs" dxfId="134" priority="142" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="143" priority="142" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:M14">
-    <cfRule type="cellIs" dxfId="133" priority="141" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="142" priority="141" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14 G14 J14:K14">
-    <cfRule type="cellIs" dxfId="132" priority="140" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="141" priority="140" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:M14">
-    <cfRule type="cellIs" dxfId="131" priority="137" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="130" priority="138" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="129" priority="139" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="140" priority="137" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="139" priority="138" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="138" priority="139" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N15">
-    <cfRule type="cellIs" dxfId="128" priority="135" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="137" priority="135" operator="greaterThan">
       <formula>$B15</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="127" priority="136" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="136" operator="equal">
       <formula>$B15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15 E15:I15 L15">
-    <cfRule type="cellIs" dxfId="126" priority="134" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="135" priority="134" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:M15">
-    <cfRule type="cellIs" dxfId="125" priority="133" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="134" priority="133" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15 G15 J15:K15">
-    <cfRule type="cellIs" dxfId="124" priority="132" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="133" priority="132" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:M15">
-    <cfRule type="cellIs" dxfId="123" priority="129" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="122" priority="130" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="121" priority="131" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="132" priority="129" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="131" priority="130" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="130" priority="131" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16:M16">
-    <cfRule type="cellIs" dxfId="120" priority="121" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="119" priority="122" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="118" priority="123" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="129" priority="121" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="128" priority="122" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="127" priority="123" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N16">
-    <cfRule type="cellIs" dxfId="117" priority="127" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="126" priority="127" operator="greaterThan">
       <formula>$B16</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="116" priority="128" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="128" operator="equal">
       <formula>$B16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16 E16:I16 L16">
-    <cfRule type="cellIs" dxfId="115" priority="126" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="124" priority="126" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16:M16">
-    <cfRule type="cellIs" dxfId="114" priority="125" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="123" priority="125" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16 G16 J16:K16">
-    <cfRule type="cellIs" dxfId="113" priority="124" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="122" priority="124" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N17">
-    <cfRule type="cellIs" dxfId="112" priority="119" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="121" priority="119" operator="greaterThan">
       <formula>$B17</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="111" priority="120" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="120" operator="equal">
       <formula>$B17</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17 E17:I17 L17">
-    <cfRule type="cellIs" dxfId="110" priority="118" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="119" priority="118" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17:M17">
-    <cfRule type="cellIs" dxfId="109" priority="117" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="118" priority="117" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D17 G17 J17:K17">
-    <cfRule type="cellIs" dxfId="108" priority="116" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="117" priority="116" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18:M18">
-    <cfRule type="cellIs" dxfId="107" priority="105" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="106" priority="106" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="105" priority="107" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="116" priority="105" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="115" priority="106" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="114" priority="107" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18 G18 J18:K18">
-    <cfRule type="cellIs" dxfId="104" priority="108" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="113" priority="108" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19:M19">
-    <cfRule type="cellIs" dxfId="103" priority="97" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="102" priority="98" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="99" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="112" priority="97" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="111" priority="98" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="110" priority="99" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N19">
-    <cfRule type="cellIs" dxfId="100" priority="103" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="109" priority="103" operator="greaterThan">
       <formula>$B19</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="99" priority="104" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="104" operator="equal">
       <formula>$B19</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19 E19:I19 L19">
-    <cfRule type="cellIs" dxfId="98" priority="102" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="107" priority="102" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19:M19">
-    <cfRule type="cellIs" dxfId="97" priority="101" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="106" priority="101" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D19 G19 J19:K19">
-    <cfRule type="cellIs" dxfId="96" priority="100" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="105" priority="100" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20:M20">
-    <cfRule type="cellIs" dxfId="95" priority="89" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="90" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="91" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="104" priority="89" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="103" priority="90" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="102" priority="91" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N20">
-    <cfRule type="cellIs" dxfId="92" priority="95" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="101" priority="95" operator="greaterThan">
       <formula>$B20</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="91" priority="96" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="96" operator="equal">
       <formula>$B20</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20 E20:I20 L20">
-    <cfRule type="cellIs" dxfId="90" priority="94" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="99" priority="94" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20:M20">
-    <cfRule type="cellIs" dxfId="89" priority="93" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="98" priority="93" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D20 G20 J20:K20">
-    <cfRule type="cellIs" dxfId="88" priority="92" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="97" priority="92" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:M21">
-    <cfRule type="cellIs" dxfId="87" priority="81" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="82" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="83" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="96" priority="81" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="95" priority="82" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="94" priority="83" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N21">
-    <cfRule type="cellIs" dxfId="84" priority="87" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="93" priority="87" operator="greaterThan">
       <formula>$B21</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="83" priority="88" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="88" operator="equal">
       <formula>$B21</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21 E21:I21 L21">
-    <cfRule type="cellIs" dxfId="82" priority="86" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="91" priority="86" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:M21">
-    <cfRule type="cellIs" dxfId="81" priority="85" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="90" priority="85" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D21 G21 J21:K21">
-    <cfRule type="cellIs" dxfId="80" priority="84" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="89" priority="84" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C25 E22:E25 G22:G25 I22:I25 L22:L25">
-    <cfRule type="cellIs" dxfId="79" priority="80" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="88" priority="80" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:M25">
-    <cfRule type="cellIs" dxfId="78" priority="79" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="87" priority="79" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:M25">
-    <cfRule type="cellIs" dxfId="77" priority="76" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="77" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="78" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="86" priority="76" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="85" priority="77" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="84" priority="78" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N22:N25">
-    <cfRule type="cellIs" dxfId="74" priority="74" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="83" priority="74" operator="greaterThan">
       <formula>$B22</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="75" operator="equal">
       <formula>$B22</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26 E26:I26 L26">
-    <cfRule type="cellIs" dxfId="72" priority="73" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="81" priority="73" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:M26">
-    <cfRule type="cellIs" dxfId="71" priority="72" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="80" priority="72" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D26 G26 J26:K26">
-    <cfRule type="cellIs" dxfId="70" priority="71" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="79" priority="71" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:M26">
-    <cfRule type="cellIs" dxfId="69" priority="68" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="69" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="70" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="78" priority="68" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="77" priority="69" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="76" priority="70" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N26">
-    <cfRule type="cellIs" dxfId="66" priority="66" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="75" priority="66" operator="greaterThan">
       <formula>$B26</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="67" operator="equal">
       <formula>$B26</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27 E27:I27 L27">
-    <cfRule type="cellIs" dxfId="64" priority="65" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="73" priority="65" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27:M27">
-    <cfRule type="cellIs" dxfId="63" priority="64" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="72" priority="64" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27 G27 J27:K27">
-    <cfRule type="cellIs" dxfId="62" priority="63" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="71" priority="63" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27:M27">
-    <cfRule type="cellIs" dxfId="61" priority="60" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="61" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="62" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="70" priority="60" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="69" priority="61" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="68" priority="62" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N27">
-    <cfRule type="cellIs" dxfId="58" priority="58" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="67" priority="58" operator="greaterThan">
       <formula>$B27</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="59" operator="equal">
       <formula>$B27</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:C39 E28:E39 G28:G39 I28:I39 L28:L39">
-    <cfRule type="cellIs" dxfId="56" priority="57" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="65" priority="57" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:M39 C28:M33">
-    <cfRule type="cellIs" dxfId="55" priority="56" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="64" priority="56" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:M39">
-    <cfRule type="cellIs" dxfId="54" priority="53" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="54" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="55" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="63" priority="53" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="62" priority="54" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="61" priority="55" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N39 N28:N30">
-    <cfRule type="cellIs" dxfId="51" priority="51" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="60" priority="51" operator="greaterThan">
       <formula>$B28</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="52" operator="equal">
       <formula>$B28</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N31:N38">
-    <cfRule type="cellIs" dxfId="49" priority="49" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="58" priority="49" operator="greaterThan">
       <formula>$B31</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="50" operator="equal">
       <formula>$B31</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40:C47 E40:E47 G40:G47 I40:I47 L40:L47">
-    <cfRule type="cellIs" dxfId="47" priority="48" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="56" priority="48" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40:M47">
-    <cfRule type="cellIs" dxfId="46" priority="47" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="55" priority="47" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40:M47">
-    <cfRule type="cellIs" dxfId="45" priority="44" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="45" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="46" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="54" priority="44" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="53" priority="45" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="46" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N43:N47">
-    <cfRule type="cellIs" dxfId="42" priority="42" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="51" priority="42" operator="greaterThan">
       <formula>$B43</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="43" operator="equal">
       <formula>$B43</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N40:N42">
-    <cfRule type="cellIs" dxfId="40" priority="40" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="49" priority="40" operator="greaterThan">
       <formula>$B40</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="41" operator="equal">
       <formula>$B40</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C51 E49:E51 G49:G51 I49:I51 L49:L51">
-    <cfRule type="cellIs" dxfId="38" priority="39" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="47" priority="39" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:M51">
-    <cfRule type="cellIs" dxfId="37" priority="38" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="46" priority="38" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:M51">
-    <cfRule type="cellIs" dxfId="36" priority="35" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="36" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="37" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="45" priority="35" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="36" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="43" priority="37" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N49:N51">
-    <cfRule type="cellIs" dxfId="33" priority="33" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="42" priority="33" operator="greaterThan">
       <formula>$B49</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="34" operator="equal">
       <formula>$B49</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48 E48:I48 L48">
-    <cfRule type="cellIs" dxfId="31" priority="32" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="40" priority="32" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:M48">
-    <cfRule type="cellIs" dxfId="30" priority="31" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="39" priority="31" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D48 G48 J48:K48">
-    <cfRule type="cellIs" dxfId="29" priority="30" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="38" priority="30" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:M48">
-    <cfRule type="cellIs" dxfId="28" priority="27" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="28" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="29" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="37" priority="27" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="28" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="35" priority="29" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N48">
-    <cfRule type="cellIs" dxfId="25" priority="25" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="34" priority="25" operator="greaterThan">
       <formula>$B48</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="26" operator="equal">
       <formula>$B48</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I55:I56">
-    <cfRule type="cellIs" dxfId="23" priority="24" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="32" priority="24" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L55 I55 G55 E55 C55">
-    <cfRule type="cellIs" dxfId="22" priority="23" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="31" priority="23" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:M55">
-    <cfRule type="cellIs" dxfId="21" priority="22" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="30" priority="22" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54:M54">
-    <cfRule type="cellIs" dxfId="20" priority="6" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="7" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="6" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="7" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="8" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N53">
-    <cfRule type="cellIs" dxfId="17" priority="20" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="26" priority="20" operator="greaterThan">
       <formula>$B53</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="21" operator="equal">
       <formula>$B53</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C53 E53:I53 L53">
-    <cfRule type="cellIs" dxfId="15" priority="19" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="24" priority="19" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C53:M53">
-    <cfRule type="cellIs" dxfId="14" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="18" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D53 G53 J53:K53">
-    <cfRule type="cellIs" dxfId="13" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="22" priority="17" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C53:M53">
-    <cfRule type="cellIs" dxfId="12" priority="14" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="15" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="14" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="15" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="16" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N54">
-    <cfRule type="cellIs" dxfId="9" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="12" operator="greaterThan">
       <formula>$B54</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="13" operator="equal">
       <formula>$B54</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54 E54:I54 L54">
-    <cfRule type="cellIs" dxfId="7" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="16" priority="11" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54:M54">
-    <cfRule type="cellIs" dxfId="6" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="10" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D54 G54 J54:K54">
-    <cfRule type="cellIs" dxfId="5" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="9" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C5">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="5" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2 C4:C5">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C5">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9159,43 +9063,43 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:L2 F24 H24:I24 C3:C20 E3:E20 G3:G20 I3:I20 K3:K20 C22:C26 G22:G26 I22:I23 I25:I26 E22:E26 K22:K26">
-    <cfRule type="cellIs" dxfId="198" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:L2 C4:L11 C13:L20 C22:L26">
-    <cfRule type="cellIs" dxfId="197" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K21 I21 G21 E21 C21">
-    <cfRule type="cellIs" dxfId="196" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:L21">
-    <cfRule type="cellIs" dxfId="195" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D25 F25 H25 J25 L25">
-    <cfRule type="cellIs" dxfId="194" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D24 G24 J24">
-    <cfRule type="cellIs" dxfId="193" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:L26">
-    <cfRule type="cellIs" dxfId="192" priority="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="191" priority="2" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="190" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Fin de journée 09/05/2019
Page avis côté client terminé.
Naviguation réparateur(utilisateur connecté) terminé.
Page A propos côté client terminé
Page A propos côté réparateur en cours(modification des informations personnelles)
</commit_message>
<xml_diff>
--- a/TPI/docs/Analyse/BJ_Planification.xlsx
+++ b/TPI/docs/Analyse/BJ_Planification.xlsx
@@ -3817,7 +3817,7 @@
   <dimension ref="A1:N59"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6127,7 +6127,7 @@
   <dimension ref="A1:N59"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6432,7 +6432,9 @@
       <c r="D12" s="4">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="E12" s="4"/>
+      <c r="E12" s="4">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
@@ -6443,7 +6445,7 @@
       <c r="M12" s="15"/>
       <c r="N12" s="3">
         <f t="shared" si="0"/>
-        <v>2.0833333333333332E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -6455,7 +6457,9 @@
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
+      <c r="E13" s="4">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
@@ -6466,7 +6470,7 @@
       <c r="M13" s="15"/>
       <c r="N13" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -6478,7 +6482,9 @@
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
+      <c r="E14" s="4">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
@@ -6489,7 +6495,7 @@
       <c r="M14" s="15"/>
       <c r="N14" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -6501,7 +6507,9 @@
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
+      <c r="E15" s="4">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
@@ -6512,7 +6520,7 @@
       <c r="M15" s="15"/>
       <c r="N15" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -6545,7 +6553,9 @@
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
+      <c r="E17" s="4">
+        <v>3.125E-2</v>
+      </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
@@ -6556,7 +6566,7 @@
       <c r="M17" s="15"/>
       <c r="N17" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.125E-2</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -6568,7 +6578,9 @@
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
+      <c r="E18" s="4">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
@@ -6579,7 +6591,7 @@
       <c r="M18" s="15"/>
       <c r="N18" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
@@ -6591,7 +6603,9 @@
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
+      <c r="E19" s="4">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
@@ -6602,7 +6616,7 @@
       <c r="M19" s="15"/>
       <c r="N19" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -7358,7 +7372,9 @@
       <c r="D53" s="4">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="E53" s="4"/>
+      <c r="E53" s="4">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="F53" s="4"/>
       <c r="G53" s="4"/>
       <c r="H53" s="4"/>
@@ -7369,7 +7385,7 @@
       <c r="M53" s="15"/>
       <c r="N53" s="3">
         <f t="shared" ref="N53:N54" si="2">SUM(C53:M53)</f>
-        <v>8.3333333333333329E-2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
@@ -7425,7 +7441,9 @@
       <c r="D56" s="13">
         <v>0.125</v>
       </c>
-      <c r="E56" s="13"/>
+      <c r="E56" s="13">
+        <v>3.125E-2</v>
+      </c>
       <c r="F56" s="13"/>
       <c r="G56" s="13"/>
       <c r="H56" s="13"/>
@@ -7436,7 +7454,7 @@
       <c r="M56" s="15"/>
       <c r="N56" s="3">
         <f>SUM(C56:M56)</f>
-        <v>0.20833333333333331</v>
+        <v>0.23958333333333331</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
@@ -7478,7 +7496,7 @@
       </c>
       <c r="E58" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.33333333333333337</v>
       </c>
       <c r="F58" s="3">
         <f t="shared" si="3"/>
@@ -7517,11 +7535,11 @@
       <c r="A59" s="42"/>
       <c r="M59" s="3">
         <f>SUM(C58:M58)</f>
-        <v>0.66666666666666674</v>
+        <v>1</v>
       </c>
       <c r="N59" s="3">
         <f>SUM(N2:N57)</f>
-        <v>0.66666666666666652</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fin de journée 13/05/2019
Page d'accueil du site côté admin terminé
Page contact côté client terminé
Début de développement de la page contact côté admin.
Suite documentation.
</commit_message>
<xml_diff>
--- a/TPI/docs/Analyse/BJ_Planification.xlsx
+++ b/TPI/docs/Analyse/BJ_Planification.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21601"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JO-PC\Documents\GitHub\TPI_Borel-Jaquet\TPI\docs\Analyse\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMINC306\Documents\GitHub\TPI_Borel-Jaquet\TPI\docs\Analyse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B933D421-AE87-4E59-B539-3D248D690404}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="690" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="690" windowWidth="19440" windowHeight="15000" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Planning prévisionnel" sheetId="1" r:id="rId1"/>
     <sheet name="Planning effectif" sheetId="5" r:id="rId2"/>
     <sheet name="Exemple" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -261,7 +260,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[hh]:mm"/>
   </numFmts>
@@ -3604,23 +3603,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -3656,23 +3638,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3848,11 +3813,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6158,11 +6123,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N59"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6639,7 +6604,7 @@
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4">
-        <v>4.1666666666666664E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
@@ -6651,7 +6616,7 @@
       <c r="M19" s="15"/>
       <c r="N19" s="3">
         <f t="shared" si="0"/>
-        <v>4.1666666666666664E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -6663,8 +6628,12 @@
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
+      <c r="E20" s="4">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="F20" s="4">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
@@ -6674,7 +6643,7 @@
       <c r="M20" s="15"/>
       <c r="N20" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.10416666666666666</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -6687,7 +6656,9 @@
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
+      <c r="F21" s="4">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
@@ -6697,7 +6668,7 @@
       <c r="M21" s="15"/>
       <c r="N21" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -6731,7 +6702,9 @@
       <c r="C23" s="4"/>
       <c r="D23" s="13"/>
       <c r="E23" s="4"/>
-      <c r="F23" s="13"/>
+      <c r="F23" s="13">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="G23" s="4"/>
       <c r="H23" s="13"/>
       <c r="I23" s="4"/>
@@ -6741,7 +6714,7 @@
       <c r="M23" s="15"/>
       <c r="N23" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -6754,7 +6727,9 @@
       <c r="C24" s="4"/>
       <c r="D24" s="13"/>
       <c r="E24" s="4"/>
-      <c r="F24" s="13"/>
+      <c r="F24" s="13">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="G24" s="4"/>
       <c r="H24" s="13"/>
       <c r="I24" s="4"/>
@@ -6764,7 +6739,7 @@
       <c r="M24" s="15"/>
       <c r="N24" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
@@ -6777,7 +6752,9 @@
       <c r="C25" s="4"/>
       <c r="D25" s="13"/>
       <c r="E25" s="4"/>
-      <c r="F25" s="13"/>
+      <c r="F25" s="13">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="G25" s="4"/>
       <c r="H25" s="13"/>
       <c r="I25" s="4"/>
@@ -6787,7 +6764,7 @@
       <c r="M25" s="15"/>
       <c r="N25" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
@@ -6823,7 +6800,9 @@
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
+      <c r="F27" s="4">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
@@ -6833,7 +6812,7 @@
       <c r="M27" s="15"/>
       <c r="N27" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
@@ -7410,7 +7389,9 @@
       <c r="E53" s="4">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="F53" s="4"/>
+      <c r="F53" s="4">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="G53" s="4"/>
       <c r="H53" s="4"/>
       <c r="I53" s="4"/>
@@ -7420,7 +7401,7 @@
       <c r="M53" s="15"/>
       <c r="N53" s="3">
         <f t="shared" ref="N53:N54" si="2">SUM(C53:M53)</f>
-        <v>0.125</v>
+        <v>0.14583333333333334</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
@@ -7479,7 +7460,9 @@
       <c r="E56" s="13">
         <v>3.125E-2</v>
       </c>
-      <c r="F56" s="13"/>
+      <c r="F56" s="13">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="G56" s="13"/>
       <c r="H56" s="13"/>
       <c r="I56" s="13"/>
@@ -7489,7 +7472,7 @@
       <c r="M56" s="15"/>
       <c r="N56" s="3">
         <f>SUM(C56:M56)</f>
-        <v>0.23958333333333331</v>
+        <v>0.28125</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
@@ -7535,7 +7518,7 @@
       </c>
       <c r="F58" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="G58" s="3">
         <f t="shared" si="3"/>
@@ -7570,11 +7553,11 @@
       <c r="A59" s="42"/>
       <c r="M59" s="3">
         <f>SUM(C58:M58)</f>
-        <v>1</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="N59" s="3">
         <f>SUM(N2:N57)</f>
-        <v>1</v>
+        <v>1.3333333333333333</v>
       </c>
     </row>
   </sheetData>
@@ -8388,7 +8371,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">

</xml_diff>

<commit_message>
Fin de journée 14/05/2019
Fin de la page demande pour l'admin
Recherche et test fullcalander.js
Début de la page avis pour l'admin (validation des avis)
</commit_message>
<xml_diff>
--- a/TPI/docs/Analyse/BJ_Planification.xlsx
+++ b/TPI/docs/Analyse/BJ_Planification.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="690" windowWidth="19440" windowHeight="15000" activeTab="1"/>
+    <workbookView xWindow="28680" yWindow="690" windowWidth="19440" windowHeight="15000"/>
   </bookViews>
   <sheets>
     <sheet name="Planning prévisionnel" sheetId="1" r:id="rId1"/>
@@ -437,7 +437,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -494,12 +494,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -512,22 +506,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -539,16 +518,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellXfs>
@@ -3816,13 +3813,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N59"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="86.7109375" style="42" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="86.7109375" style="40" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
     <col min="3" max="13" width="11.5703125" customWidth="1"/>
   </cols>
@@ -3897,7 +3894,7 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="41" t="s">
         <v>40</v>
       </c>
       <c r="B3" s="34">
@@ -3922,28 +3919,28 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="55" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="15"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="21"/>
       <c r="N4" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="42" t="s">
+      <c r="A5" s="40" t="s">
         <v>44</v>
       </c>
       <c r="B5" s="34">
@@ -3968,28 +3965,28 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="15"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="21"/>
       <c r="N6" s="3">
         <f t="shared" ref="N6:N48" si="1">SUM(C6:M6)</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="43" t="s">
         <v>46</v>
       </c>
       <c r="B7" s="34">
@@ -4014,7 +4011,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="43" t="s">
         <v>47</v>
       </c>
       <c r="B8" s="34">
@@ -4039,7 +4036,7 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="45" t="s">
+      <c r="A9" s="43" t="s">
         <v>77</v>
       </c>
       <c r="B9" s="34">
@@ -4064,7 +4061,7 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="43" t="s">
         <v>43</v>
       </c>
       <c r="B10" s="34">
@@ -4089,28 +4086,28 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="48" t="s">
+      <c r="A11" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="34"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="15"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="22"/>
+      <c r="M11" s="21"/>
       <c r="N11" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="45" t="s">
+      <c r="A12" s="43" t="s">
         <v>46</v>
       </c>
       <c r="B12" s="34">
@@ -4137,7 +4134,7 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="45" t="s">
+      <c r="A13" s="43" t="s">
         <v>50</v>
       </c>
       <c r="B13" s="34">
@@ -4162,7 +4159,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="45" t="s">
+      <c r="A14" s="43" t="s">
         <v>51</v>
       </c>
       <c r="B14" s="34">
@@ -4187,7 +4184,7 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="45" t="s">
+      <c r="A15" s="43" t="s">
         <v>43</v>
       </c>
       <c r="B15" s="34">
@@ -4212,28 +4209,28 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="48" t="s">
+      <c r="A16" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="34"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="15"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="22"/>
+      <c r="L16" s="22"/>
+      <c r="M16" s="21"/>
       <c r="N16" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="45" t="s">
+      <c r="A17" s="43" t="s">
         <v>46</v>
       </c>
       <c r="B17" s="34">
@@ -4258,7 +4255,7 @@
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="45" t="s">
+      <c r="A18" s="43" t="s">
         <v>53</v>
       </c>
       <c r="B18" s="34">
@@ -4283,7 +4280,7 @@
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="45" t="s">
+      <c r="A19" s="43" t="s">
         <v>54</v>
       </c>
       <c r="B19" s="34">
@@ -4308,7 +4305,7 @@
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="45" t="s">
+      <c r="A20" s="43" t="s">
         <v>55</v>
       </c>
       <c r="B20" s="34">
@@ -4333,7 +4330,7 @@
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="45" t="s">
+      <c r="A21" s="43" t="s">
         <v>43</v>
       </c>
       <c r="B21" s="34">
@@ -4358,28 +4355,28 @@
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="48" t="s">
+      <c r="A22" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="B22" s="34"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="15"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="20"/>
+      <c r="L22" s="22"/>
+      <c r="M22" s="21"/>
       <c r="N22" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="49" t="s">
+      <c r="A23" s="44" t="s">
         <v>46</v>
       </c>
       <c r="B23" s="34">
@@ -4404,7 +4401,7 @@
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="45" t="s">
+      <c r="A24" s="43" t="s">
         <v>57</v>
       </c>
       <c r="B24" s="34">
@@ -4431,7 +4428,7 @@
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="49" t="s">
+      <c r="A25" s="44" t="s">
         <v>58</v>
       </c>
       <c r="B25" s="34">
@@ -4456,7 +4453,7 @@
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="45" t="s">
+      <c r="A26" s="43" t="s">
         <v>59</v>
       </c>
       <c r="B26" s="34">
@@ -4481,7 +4478,7 @@
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="49" t="s">
+      <c r="A27" s="44" t="s">
         <v>43</v>
       </c>
       <c r="B27" s="34">
@@ -4509,46 +4506,46 @@
       <c r="A28" s="50" t="s">
         <v>60</v>
       </c>
-      <c r="B28" s="34"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="13"/>
-      <c r="K28" s="13"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="15"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="20"/>
+      <c r="K28" s="20"/>
+      <c r="L28" s="22"/>
+      <c r="M28" s="21"/>
       <c r="N28" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="51" t="s">
+      <c r="A29" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="B29" s="34"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="13"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="13"/>
-      <c r="K29" s="13"/>
-      <c r="L29" s="4"/>
-      <c r="M29" s="15"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="22"/>
+      <c r="J29" s="20"/>
+      <c r="K29" s="20"/>
+      <c r="L29" s="22"/>
+      <c r="M29" s="21"/>
       <c r="N29" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="52" t="s">
+      <c r="A30" s="45" t="s">
         <v>46</v>
       </c>
       <c r="B30" s="34">
@@ -4573,11 +4570,11 @@
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="53" t="s">
+      <c r="A31" s="46" t="s">
         <v>76</v>
       </c>
       <c r="B31" s="34">
-        <v>4.1666666666666664E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="C31" s="4"/>
       <c r="D31" s="13"/>
@@ -4598,7 +4595,7 @@
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="53" t="s">
+      <c r="A32" s="46" t="s">
         <v>75</v>
       </c>
       <c r="B32" s="34">
@@ -4623,7 +4620,7 @@
       </c>
     </row>
     <row r="33" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="54" t="s">
+      <c r="A33" s="47" t="s">
         <v>62</v>
       </c>
       <c r="B33" s="34">
@@ -4648,7 +4645,7 @@
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="52" t="s">
+      <c r="A34" s="45" t="s">
         <v>43</v>
       </c>
       <c r="B34" s="34">
@@ -4673,28 +4670,28 @@
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="51" t="s">
+      <c r="A35" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="B35" s="34"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="13"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="13"/>
-      <c r="K35" s="13"/>
-      <c r="L35" s="1"/>
-      <c r="M35" s="15"/>
+      <c r="B35" s="32"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="20"/>
+      <c r="I35" s="19"/>
+      <c r="J35" s="20"/>
+      <c r="K35" s="20"/>
+      <c r="L35" s="19"/>
+      <c r="M35" s="21"/>
       <c r="N35" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="52" t="s">
+      <c r="A36" s="45" t="s">
         <v>46</v>
       </c>
       <c r="B36" s="34">
@@ -4719,7 +4716,7 @@
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" s="53" t="s">
+      <c r="A37" s="46" t="s">
         <v>63</v>
       </c>
       <c r="B37" s="34">
@@ -4744,7 +4741,7 @@
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" s="53" t="s">
+      <c r="A38" s="46" t="s">
         <v>64</v>
       </c>
       <c r="B38" s="34">
@@ -4769,7 +4766,7 @@
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" s="52" t="s">
+      <c r="A39" s="45" t="s">
         <v>43</v>
       </c>
       <c r="B39" s="34">
@@ -4797,25 +4794,25 @@
       <c r="A40" s="56" t="s">
         <v>65</v>
       </c>
-      <c r="B40" s="34"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="13"/>
-      <c r="G40" s="4"/>
-      <c r="H40" s="13"/>
-      <c r="I40" s="4"/>
-      <c r="J40" s="13"/>
-      <c r="K40" s="13"/>
-      <c r="L40" s="4"/>
-      <c r="M40" s="15"/>
+      <c r="B40" s="32"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="22"/>
+      <c r="H40" s="20"/>
+      <c r="I40" s="22"/>
+      <c r="J40" s="20"/>
+      <c r="K40" s="20"/>
+      <c r="L40" s="22"/>
+      <c r="M40" s="21"/>
       <c r="N40" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A41" s="52" t="s">
+      <c r="A41" s="45" t="s">
         <v>46</v>
       </c>
       <c r="B41" s="34">
@@ -4840,7 +4837,7 @@
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A42" s="52" t="s">
+      <c r="A42" s="45" t="s">
         <v>66</v>
       </c>
       <c r="B42" s="34">
@@ -4867,7 +4864,7 @@
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" s="54" t="s">
+      <c r="A43" s="47" t="s">
         <v>67</v>
       </c>
       <c r="B43" s="34">
@@ -4892,7 +4889,7 @@
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A44" s="53" t="s">
+      <c r="A44" s="46" t="s">
         <v>68</v>
       </c>
       <c r="B44" s="34">
@@ -4917,7 +4914,7 @@
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" s="52" t="s">
+      <c r="A45" s="45" t="s">
         <v>69</v>
       </c>
       <c r="B45" s="34">
@@ -4942,7 +4939,7 @@
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A46" s="57" t="s">
+      <c r="A46" s="48" t="s">
         <v>70</v>
       </c>
       <c r="B46" s="34">
@@ -4967,7 +4964,7 @@
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A47" s="53" t="s">
+      <c r="A47" s="46" t="s">
         <v>43</v>
       </c>
       <c r="B47" s="34">
@@ -4992,28 +4989,28 @@
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A48" s="58" t="s">
+      <c r="A48" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="B48" s="34"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="4"/>
-      <c r="G48" s="4"/>
-      <c r="H48" s="4"/>
-      <c r="I48" s="4"/>
-      <c r="J48" s="4"/>
-      <c r="K48" s="4"/>
-      <c r="L48" s="4"/>
-      <c r="M48" s="15"/>
+      <c r="B48" s="32"/>
+      <c r="C48" s="22"/>
+      <c r="D48" s="22"/>
+      <c r="E48" s="22"/>
+      <c r="F48" s="22"/>
+      <c r="G48" s="22"/>
+      <c r="H48" s="22"/>
+      <c r="I48" s="22"/>
+      <c r="J48" s="22"/>
+      <c r="K48" s="22"/>
+      <c r="L48" s="22"/>
+      <c r="M48" s="21"/>
       <c r="N48" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A49" s="52" t="s">
+      <c r="A49" s="45" t="s">
         <v>46</v>
       </c>
       <c r="B49" s="34">
@@ -5038,7 +5035,7 @@
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A50" s="57" t="s">
+      <c r="A50" s="48" t="s">
         <v>72</v>
       </c>
       <c r="B50" s="34">
@@ -5063,7 +5060,7 @@
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A51" s="57" t="s">
+      <c r="A51" s="48" t="s">
         <v>43</v>
       </c>
       <c r="B51" s="34">
@@ -5088,23 +5085,23 @@
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A52" s="45"/>
-      <c r="B52" s="34"/>
-      <c r="C52" s="4"/>
-      <c r="D52" s="4"/>
-      <c r="E52" s="4"/>
-      <c r="F52" s="4"/>
-      <c r="G52" s="4"/>
-      <c r="H52" s="4"/>
-      <c r="I52" s="4"/>
-      <c r="J52" s="4"/>
-      <c r="K52" s="4"/>
-      <c r="L52" s="4"/>
-      <c r="M52" s="15"/>
+      <c r="A52" s="52"/>
+      <c r="B52" s="32"/>
+      <c r="C52" s="22"/>
+      <c r="D52" s="22"/>
+      <c r="E52" s="22"/>
+      <c r="F52" s="22"/>
+      <c r="G52" s="22"/>
+      <c r="H52" s="22"/>
+      <c r="I52" s="22"/>
+      <c r="J52" s="22"/>
+      <c r="K52" s="22"/>
+      <c r="L52" s="22"/>
+      <c r="M52" s="21"/>
       <c r="N52" s="3"/>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A53" s="44" t="s">
+      <c r="A53" s="42" t="s">
         <v>73</v>
       </c>
       <c r="B53" s="34">
@@ -5143,47 +5140,47 @@
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A54" s="41"/>
-      <c r="B54" s="34"/>
-      <c r="C54" s="4"/>
-      <c r="D54" s="4"/>
-      <c r="E54" s="4"/>
-      <c r="F54" s="4"/>
-      <c r="G54" s="4"/>
-      <c r="H54" s="4"/>
-      <c r="I54" s="4"/>
-      <c r="J54" s="4"/>
-      <c r="K54" s="4"/>
-      <c r="L54" s="4"/>
-      <c r="M54" s="15"/>
+      <c r="A54" s="53"/>
+      <c r="B54" s="32"/>
+      <c r="C54" s="22"/>
+      <c r="D54" s="22"/>
+      <c r="E54" s="22"/>
+      <c r="F54" s="22"/>
+      <c r="G54" s="22"/>
+      <c r="H54" s="22"/>
+      <c r="I54" s="22"/>
+      <c r="J54" s="22"/>
+      <c r="K54" s="22"/>
+      <c r="L54" s="22"/>
+      <c r="M54" s="21"/>
       <c r="N54" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A55" s="44" t="s">
+      <c r="A55" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B55" s="34"/>
-      <c r="C55" s="4"/>
-      <c r="D55" s="13"/>
-      <c r="E55" s="4"/>
-      <c r="F55" s="13"/>
-      <c r="G55" s="4"/>
-      <c r="H55" s="13"/>
-      <c r="I55" s="4"/>
-      <c r="J55" s="13"/>
-      <c r="K55" s="13"/>
-      <c r="L55" s="4"/>
-      <c r="M55" s="15"/>
+      <c r="B55" s="32"/>
+      <c r="C55" s="22"/>
+      <c r="D55" s="20"/>
+      <c r="E55" s="22"/>
+      <c r="F55" s="20"/>
+      <c r="G55" s="22"/>
+      <c r="H55" s="20"/>
+      <c r="I55" s="22"/>
+      <c r="J55" s="20"/>
+      <c r="K55" s="20"/>
+      <c r="L55" s="22"/>
+      <c r="M55" s="21"/>
       <c r="N55" s="3">
         <f>SUM(C55:M55)</f>
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A56" s="45" t="s">
+      <c r="A56" s="43" t="s">
         <v>74</v>
       </c>
       <c r="B56" s="34">
@@ -5228,7 +5225,7 @@
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A57" s="45" t="s">
+      <c r="A57" s="43" t="s">
         <v>42</v>
       </c>
       <c r="B57" s="34">
@@ -5255,7 +5252,7 @@
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B58" s="3">
         <f t="shared" ref="B58:M58" si="4">SUM(B2:B57)</f>
-        <v>3.6249999999999996</v>
+        <v>3.6666666666666661</v>
       </c>
       <c r="C58" s="3">
         <f t="shared" si="4"/>
@@ -6126,13 +6123,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I48" sqref="I48"/>
+    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="59.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="87.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
     <col min="3" max="13" width="11.5703125" customWidth="1"/>
   </cols>
@@ -6207,7 +6204,7 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="41" t="s">
         <v>40</v>
       </c>
       <c r="B3" s="34">
@@ -6232,28 +6229,28 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="55" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="15"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="21"/>
       <c r="N4" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="42" t="s">
+      <c r="A5" s="40" t="s">
         <v>44</v>
       </c>
       <c r="B5" s="34">
@@ -6280,28 +6277,28 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="15"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="21"/>
       <c r="N6" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="43" t="s">
         <v>46</v>
       </c>
       <c r="B7" s="34">
@@ -6326,7 +6323,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="43" t="s">
         <v>47</v>
       </c>
       <c r="B8" s="34">
@@ -6351,7 +6348,7 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="45" t="s">
+      <c r="A9" s="43" t="s">
         <v>48</v>
       </c>
       <c r="B9" s="34">
@@ -6376,7 +6373,7 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="43" t="s">
         <v>43</v>
       </c>
       <c r="B10" s="34">
@@ -6401,28 +6398,28 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="48" t="s">
+      <c r="A11" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="34"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="15"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="22"/>
+      <c r="M11" s="21"/>
       <c r="N11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="45" t="s">
+      <c r="A12" s="43" t="s">
         <v>46</v>
       </c>
       <c r="B12" s="34">
@@ -6449,7 +6446,7 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="45" t="s">
+      <c r="A13" s="43" t="s">
         <v>50</v>
       </c>
       <c r="B13" s="34">
@@ -6474,7 +6471,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="45" t="s">
+      <c r="A14" s="43" t="s">
         <v>51</v>
       </c>
       <c r="B14" s="34">
@@ -6499,7 +6496,7 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="45" t="s">
+      <c r="A15" s="43" t="s">
         <v>43</v>
       </c>
       <c r="B15" s="34">
@@ -6524,28 +6521,28 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="48" t="s">
+      <c r="A16" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="34"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="15"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="22"/>
+      <c r="L16" s="22"/>
+      <c r="M16" s="21"/>
       <c r="N16" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="45" t="s">
+      <c r="A17" s="43" t="s">
         <v>46</v>
       </c>
       <c r="B17" s="34">
@@ -6570,7 +6567,7 @@
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="45" t="s">
+      <c r="A18" s="43" t="s">
         <v>53</v>
       </c>
       <c r="B18" s="34">
@@ -6595,7 +6592,7 @@
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="45" t="s">
+      <c r="A19" s="43" t="s">
         <v>54</v>
       </c>
       <c r="B19" s="34">
@@ -6620,7 +6617,7 @@
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="45" t="s">
+      <c r="A20" s="43" t="s">
         <v>55</v>
       </c>
       <c r="B20" s="34">
@@ -6632,7 +6629,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="F20" s="4">
-        <v>8.3333333333333329E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
@@ -6643,11 +6640,11 @@
       <c r="M20" s="15"/>
       <c r="N20" s="3">
         <f t="shared" si="0"/>
-        <v>0.10416666666666666</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="45" t="s">
+      <c r="A21" s="43" t="s">
         <v>43</v>
       </c>
       <c r="B21" s="34">
@@ -6672,28 +6669,28 @@
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="48" t="s">
+      <c r="A22" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="B22" s="34"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="15"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="20"/>
+      <c r="L22" s="22"/>
+      <c r="M22" s="21"/>
       <c r="N22" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="49" t="s">
+      <c r="A23" s="44" t="s">
         <v>46</v>
       </c>
       <c r="B23" s="34">
@@ -6718,7 +6715,7 @@
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="45" t="s">
+      <c r="A24" s="43" t="s">
         <v>57</v>
       </c>
       <c r="B24" s="34">
@@ -6743,7 +6740,7 @@
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="49" t="s">
+      <c r="A25" s="44" t="s">
         <v>58</v>
       </c>
       <c r="B25" s="34">
@@ -6768,7 +6765,7 @@
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="45" t="s">
+      <c r="A26" s="43" t="s">
         <v>59</v>
       </c>
       <c r="B26" s="34">
@@ -6791,7 +6788,7 @@
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="49" t="s">
+      <c r="A27" s="44" t="s">
         <v>43</v>
       </c>
       <c r="B27" s="34">
@@ -6819,46 +6816,46 @@
       <c r="A28" s="50" t="s">
         <v>60</v>
       </c>
-      <c r="B28" s="34"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="13"/>
-      <c r="K28" s="13"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="15"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="20"/>
+      <c r="K28" s="20"/>
+      <c r="L28" s="22"/>
+      <c r="M28" s="21"/>
       <c r="N28" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="51" t="s">
+      <c r="A29" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="B29" s="34"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="13"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="13"/>
-      <c r="K29" s="13"/>
-      <c r="L29" s="4"/>
-      <c r="M29" s="15"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="22"/>
+      <c r="J29" s="20"/>
+      <c r="K29" s="20"/>
+      <c r="L29" s="22"/>
+      <c r="M29" s="21"/>
       <c r="N29" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="52" t="s">
+      <c r="A30" s="45" t="s">
         <v>46</v>
       </c>
       <c r="B30" s="34">
@@ -6867,7 +6864,9 @@
       <c r="C30" s="4"/>
       <c r="D30" s="13"/>
       <c r="E30" s="4"/>
-      <c r="F30" s="13"/>
+      <c r="F30" s="13">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="G30" s="4"/>
       <c r="H30" s="13"/>
       <c r="I30" s="4"/>
@@ -6877,11 +6876,11 @@
       <c r="M30" s="15"/>
       <c r="N30" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="53" t="s">
+      <c r="A31" s="46" t="s">
         <v>76</v>
       </c>
       <c r="B31" s="34">
@@ -6890,8 +6889,12 @@
       <c r="C31" s="4"/>
       <c r="D31" s="13"/>
       <c r="E31" s="4"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="4"/>
+      <c r="F31" s="13">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="G31" s="4">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="H31" s="13"/>
       <c r="I31" s="1"/>
       <c r="J31" s="13"/>
@@ -6900,11 +6903,11 @@
       <c r="M31" s="15"/>
       <c r="N31" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="53" t="s">
+      <c r="A32" s="46" t="s">
         <v>75</v>
       </c>
       <c r="B32" s="34">
@@ -6914,7 +6917,9 @@
       <c r="D32" s="13"/>
       <c r="E32" s="4"/>
       <c r="F32" s="13"/>
-      <c r="G32" s="4"/>
+      <c r="G32" s="4">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="H32" s="13"/>
       <c r="I32" s="1"/>
       <c r="J32" s="13"/>
@@ -6923,11 +6928,11 @@
       <c r="M32" s="15"/>
       <c r="N32" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="54" t="s">
+      <c r="A33" s="47" t="s">
         <v>62</v>
       </c>
       <c r="B33" s="34">
@@ -6950,7 +6955,7 @@
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="52" t="s">
+      <c r="A34" s="45" t="s">
         <v>43</v>
       </c>
       <c r="B34" s="34">
@@ -6960,7 +6965,9 @@
       <c r="D34" s="13"/>
       <c r="E34" s="4"/>
       <c r="F34" s="13"/>
-      <c r="G34" s="1"/>
+      <c r="G34" s="4">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="H34" s="13"/>
       <c r="I34" s="4"/>
       <c r="J34" s="13"/>
@@ -6969,32 +6976,32 @@
       <c r="M34" s="15"/>
       <c r="N34" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="51" t="s">
+      <c r="A35" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="B35" s="34"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="13"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="13"/>
-      <c r="K35" s="13"/>
-      <c r="L35" s="1"/>
-      <c r="M35" s="15"/>
+      <c r="B35" s="32"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="20"/>
+      <c r="I35" s="19"/>
+      <c r="J35" s="20"/>
+      <c r="K35" s="20"/>
+      <c r="L35" s="19"/>
+      <c r="M35" s="21"/>
       <c r="N35" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="52" t="s">
+      <c r="A36" s="45" t="s">
         <v>46</v>
       </c>
       <c r="B36" s="34">
@@ -7004,7 +7011,9 @@
       <c r="D36" s="13"/>
       <c r="E36" s="4"/>
       <c r="F36" s="13"/>
-      <c r="G36" s="24"/>
+      <c r="G36" s="4">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="H36" s="13"/>
       <c r="I36" s="37"/>
       <c r="J36" s="13"/>
@@ -7013,11 +7022,11 @@
       <c r="M36" s="15"/>
       <c r="N36" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" s="53" t="s">
+      <c r="A37" s="46" t="s">
         <v>63</v>
       </c>
       <c r="B37" s="34">
@@ -7027,7 +7036,9 @@
       <c r="D37" s="13"/>
       <c r="E37" s="4"/>
       <c r="F37" s="13"/>
-      <c r="G37" s="4"/>
+      <c r="G37" s="4">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="H37" s="13"/>
       <c r="I37" s="4"/>
       <c r="J37" s="13"/>
@@ -7036,11 +7047,11 @@
       <c r="M37" s="15"/>
       <c r="N37" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" s="53" t="s">
+      <c r="A38" s="46" t="s">
         <v>64</v>
       </c>
       <c r="B38" s="34">
@@ -7063,7 +7074,7 @@
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" s="52" t="s">
+      <c r="A39" s="45" t="s">
         <v>43</v>
       </c>
       <c r="B39" s="34">
@@ -7086,28 +7097,28 @@
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" s="55" t="s">
+      <c r="A40" s="56" t="s">
         <v>65</v>
       </c>
-      <c r="B40" s="34"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="13"/>
-      <c r="G40" s="4"/>
-      <c r="H40" s="13"/>
-      <c r="I40" s="4"/>
-      <c r="J40" s="13"/>
-      <c r="K40" s="13"/>
-      <c r="L40" s="4"/>
-      <c r="M40" s="15"/>
+      <c r="B40" s="32"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="22"/>
+      <c r="H40" s="20"/>
+      <c r="I40" s="22"/>
+      <c r="J40" s="20"/>
+      <c r="K40" s="20"/>
+      <c r="L40" s="22"/>
+      <c r="M40" s="21"/>
       <c r="N40" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A41" s="49" t="s">
+      <c r="A41" s="45" t="s">
         <v>46</v>
       </c>
       <c r="B41" s="34">
@@ -7130,7 +7141,7 @@
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A42" s="49" t="s">
+      <c r="A42" s="45" t="s">
         <v>66</v>
       </c>
       <c r="B42" s="34">
@@ -7199,7 +7210,7 @@
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" s="49" t="s">
+      <c r="A45" s="45" t="s">
         <v>69</v>
       </c>
       <c r="B45" s="34">
@@ -7222,7 +7233,7 @@
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A46" s="45" t="s">
+      <c r="A46" s="48" t="s">
         <v>70</v>
       </c>
       <c r="B46" s="34">
@@ -7268,28 +7279,28 @@
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A48" s="48" t="s">
+      <c r="A48" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="B48" s="34"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="4"/>
-      <c r="G48" s="4"/>
-      <c r="H48" s="4"/>
-      <c r="I48" s="4"/>
-      <c r="J48" s="4"/>
-      <c r="K48" s="4"/>
-      <c r="L48" s="4"/>
-      <c r="M48" s="15"/>
+      <c r="B48" s="32"/>
+      <c r="C48" s="22"/>
+      <c r="D48" s="22"/>
+      <c r="E48" s="22"/>
+      <c r="F48" s="22"/>
+      <c r="G48" s="22"/>
+      <c r="H48" s="22"/>
+      <c r="I48" s="22"/>
+      <c r="J48" s="22"/>
+      <c r="K48" s="22"/>
+      <c r="L48" s="22"/>
+      <c r="M48" s="21"/>
       <c r="N48" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A49" s="49" t="s">
+      <c r="A49" s="45" t="s">
         <v>46</v>
       </c>
       <c r="B49" s="34">
@@ -7312,7 +7323,7 @@
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A50" s="45" t="s">
+      <c r="A50" s="48" t="s">
         <v>72</v>
       </c>
       <c r="B50" s="34">
@@ -7335,7 +7346,7 @@
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A51" s="45" t="s">
+      <c r="A51" s="48" t="s">
         <v>43</v>
       </c>
       <c r="B51" s="34">
@@ -7358,23 +7369,23 @@
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A52" s="45"/>
-      <c r="B52" s="34"/>
-      <c r="C52" s="4"/>
-      <c r="D52" s="4"/>
-      <c r="E52" s="4"/>
-      <c r="F52" s="4"/>
-      <c r="G52" s="4"/>
-      <c r="H52" s="4"/>
-      <c r="I52" s="4"/>
-      <c r="J52" s="4"/>
-      <c r="K52" s="4"/>
-      <c r="L52" s="4"/>
-      <c r="M52" s="15"/>
+      <c r="A52" s="52"/>
+      <c r="B52" s="32"/>
+      <c r="C52" s="22"/>
+      <c r="D52" s="22"/>
+      <c r="E52" s="22"/>
+      <c r="F52" s="22"/>
+      <c r="G52" s="22"/>
+      <c r="H52" s="22"/>
+      <c r="I52" s="22"/>
+      <c r="J52" s="22"/>
+      <c r="K52" s="22"/>
+      <c r="L52" s="22"/>
+      <c r="M52" s="21"/>
       <c r="N52" s="3"/>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A53" s="44" t="s">
+      <c r="A53" s="42" t="s">
         <v>73</v>
       </c>
       <c r="B53" s="34">
@@ -7392,7 +7403,9 @@
       <c r="F53" s="4">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="G53" s="4"/>
+      <c r="G53" s="4">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="H53" s="4"/>
       <c r="I53" s="4"/>
       <c r="J53" s="4"/>
@@ -7401,51 +7414,51 @@
       <c r="M53" s="15"/>
       <c r="N53" s="3">
         <f t="shared" ref="N53:N54" si="2">SUM(C53:M53)</f>
-        <v>0.14583333333333334</v>
+        <v>0.1875</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A54" s="41"/>
-      <c r="B54" s="34"/>
-      <c r="C54" s="4"/>
-      <c r="D54" s="4"/>
-      <c r="E54" s="4"/>
-      <c r="F54" s="4"/>
-      <c r="G54" s="4"/>
-      <c r="H54" s="4"/>
-      <c r="I54" s="4"/>
-      <c r="J54" s="4"/>
-      <c r="K54" s="4"/>
-      <c r="L54" s="4"/>
-      <c r="M54" s="15"/>
+      <c r="A54" s="53"/>
+      <c r="B54" s="32"/>
+      <c r="C54" s="22"/>
+      <c r="D54" s="22"/>
+      <c r="E54" s="22"/>
+      <c r="F54" s="22"/>
+      <c r="G54" s="22"/>
+      <c r="H54" s="22"/>
+      <c r="I54" s="22"/>
+      <c r="J54" s="22"/>
+      <c r="K54" s="22"/>
+      <c r="L54" s="22"/>
+      <c r="M54" s="21"/>
       <c r="N54" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A55" s="44" t="s">
+      <c r="A55" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B55" s="34"/>
-      <c r="C55" s="4"/>
-      <c r="D55" s="13"/>
-      <c r="E55" s="4"/>
-      <c r="F55" s="13"/>
-      <c r="G55" s="4"/>
-      <c r="H55" s="13"/>
-      <c r="I55" s="4"/>
-      <c r="J55" s="13"/>
-      <c r="K55" s="13"/>
-      <c r="L55" s="4"/>
-      <c r="M55" s="15"/>
+      <c r="B55" s="32"/>
+      <c r="C55" s="22"/>
+      <c r="D55" s="20"/>
+      <c r="E55" s="22"/>
+      <c r="F55" s="20"/>
+      <c r="G55" s="22"/>
+      <c r="H55" s="20"/>
+      <c r="I55" s="22"/>
+      <c r="J55" s="20"/>
+      <c r="K55" s="20"/>
+      <c r="L55" s="22"/>
+      <c r="M55" s="21"/>
       <c r="N55" s="3">
         <f>SUM(C55:M55)</f>
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A56" s="45" t="s">
+      <c r="A56" s="43" t="s">
         <v>74</v>
       </c>
       <c r="B56" s="34">
@@ -7463,7 +7476,9 @@
       <c r="F56" s="13">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="G56" s="13"/>
+      <c r="G56" s="13">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="H56" s="13"/>
       <c r="I56" s="13"/>
       <c r="J56" s="13"/>
@@ -7472,11 +7487,11 @@
       <c r="M56" s="15"/>
       <c r="N56" s="3">
         <f>SUM(C56:M56)</f>
-        <v>0.28125</v>
+        <v>0.36458333333333331</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A57" s="45" t="s">
+      <c r="A57" s="43" t="s">
         <v>42</v>
       </c>
       <c r="B57" s="34">
@@ -7499,7 +7514,7 @@
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A58" s="42"/>
+      <c r="A58" s="40"/>
       <c r="B58" s="3">
         <f t="shared" ref="B58:M58" si="3">SUM(B2:B57)</f>
         <v>3.6249999999999996</v>
@@ -7522,7 +7537,7 @@
       </c>
       <c r="G58" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="H58" s="3">
         <f t="shared" si="3"/>
@@ -7550,14 +7565,14 @@
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A59" s="42"/>
+      <c r="A59" s="40"/>
       <c r="M59" s="3">
         <f>SUM(C58:M58)</f>
-        <v>1.3333333333333333</v>
+        <v>1.6666666666666665</v>
       </c>
       <c r="N59" s="3">
         <f>SUM(N2:N57)</f>
-        <v>1.3333333333333333</v>
+        <v>1.6666666666666667</v>
       </c>
     </row>
   </sheetData>
@@ -8124,12 +8139,12 @@
       <formula>$B27</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C28:C39 E28:E39 G28:G39 I28:I39 L28:L39">
+  <conditionalFormatting sqref="C28:C39 E28:E39 I28:I39 L28:L39 G28:G39">
     <cfRule type="cellIs" dxfId="65" priority="57" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C35:M39 C28:M33">
+  <conditionalFormatting sqref="C28:M33 C35:M39">
     <cfRule type="cellIs" dxfId="64" priority="56" operator="greaterThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Fin de journée 15/05/2019
Suite de documentation
Suite et fin du développement de la page avis côté administrateur
</commit_message>
<xml_diff>
--- a/TPI/docs/Analyse/BJ_Planification.xlsx
+++ b/TPI/docs/Analyse/BJ_Planification.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="690" windowWidth="19440" windowHeight="15000"/>
+    <workbookView xWindow="28680" yWindow="690" windowWidth="19440" windowHeight="15000" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Planning prévisionnel" sheetId="1" r:id="rId1"/>
@@ -3813,7 +3813,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
@@ -6123,8 +6123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N59"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7039,7 +7039,9 @@
       <c r="G37" s="4">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="H37" s="13"/>
+      <c r="H37" s="13">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="I37" s="4"/>
       <c r="J37" s="13"/>
       <c r="K37" s="13"/>
@@ -7047,7 +7049,7 @@
       <c r="M37" s="15"/>
       <c r="N37" s="3">
         <f t="shared" si="0"/>
-        <v>4.1666666666666664E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
@@ -7062,7 +7064,9 @@
       <c r="E38" s="4"/>
       <c r="F38" s="13"/>
       <c r="G38" s="4"/>
-      <c r="H38" s="13"/>
+      <c r="H38" s="13">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="I38" s="4"/>
       <c r="J38" s="13"/>
       <c r="K38" s="13"/>
@@ -7070,7 +7074,7 @@
       <c r="M38" s="15"/>
       <c r="N38" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
@@ -7085,7 +7089,9 @@
       <c r="E39" s="4"/>
       <c r="F39" s="13"/>
       <c r="G39" s="4"/>
-      <c r="H39" s="13"/>
+      <c r="H39" s="13">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="I39" s="4"/>
       <c r="J39" s="13"/>
       <c r="K39" s="13"/>
@@ -7093,7 +7099,7 @@
       <c r="M39" s="15"/>
       <c r="N39" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
@@ -7406,7 +7412,9 @@
       <c r="G53" s="4">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="H53" s="4"/>
+      <c r="H53" s="4">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="I53" s="4"/>
       <c r="J53" s="4"/>
       <c r="K53" s="4"/>
@@ -7414,7 +7422,7 @@
       <c r="M53" s="15"/>
       <c r="N53" s="3">
         <f t="shared" ref="N53:N54" si="2">SUM(C53:M53)</f>
-        <v>0.1875</v>
+        <v>0.22916666666666666</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
@@ -7479,7 +7487,9 @@
       <c r="G56" s="13">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="H56" s="13"/>
+      <c r="H56" s="13">
+        <v>0.16666666666666666</v>
+      </c>
       <c r="I56" s="13"/>
       <c r="J56" s="13"/>
       <c r="K56" s="13"/>
@@ -7487,7 +7497,7 @@
       <c r="M56" s="15"/>
       <c r="N56" s="3">
         <f>SUM(C56:M56)</f>
-        <v>0.36458333333333331</v>
+        <v>0.53125</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
@@ -7541,7 +7551,7 @@
       </c>
       <c r="H58" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="I58" s="3">
         <f t="shared" si="3"/>
@@ -7568,11 +7578,11 @@
       <c r="A59" s="40"/>
       <c r="M59" s="3">
         <f>SUM(C58:M58)</f>
-        <v>1.6666666666666665</v>
+        <v>1.9999999999999998</v>
       </c>
       <c r="N59" s="3">
         <f>SUM(N2:N57)</f>
-        <v>1.6666666666666667</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fin de journée 20/05/2019
Modification de la base de données (table "evenement" modifié)
Modification des fonctions utilisant la table "evenement".
Suite de la page calendrier (FullCalendar)
Documentation (suite aux commentaires de M.Travnjak
</commit_message>
<xml_diff>
--- a/TPI/docs/Analyse/BJ_Planification.xlsx
+++ b/TPI/docs/Analyse/BJ_Planification.xlsx
@@ -3813,7 +3813,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N59"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
@@ -6123,8 +6123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7506,10 +7506,12 @@
       <c r="J56" s="13"/>
       <c r="K56" s="13"/>
       <c r="L56" s="13"/>
-      <c r="M56" s="15"/>
+      <c r="M56" s="15">
+        <v>0.25</v>
+      </c>
       <c r="N56" s="3">
         <f>SUM(C56:M56)</f>
-        <v>0.57291666666666663</v>
+        <v>0.82291666666666663</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
@@ -7529,10 +7531,12 @@
       <c r="J57" s="4"/>
       <c r="K57" s="4"/>
       <c r="L57" s="4"/>
-      <c r="M57" s="15"/>
+      <c r="M57" s="15">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="N57" s="3">
         <f>SUM(C57:M57)</f>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
@@ -7583,18 +7587,18 @@
       </c>
       <c r="M58" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="40"/>
       <c r="M59" s="3">
         <f>SUM(C58:M58)</f>
-        <v>2.333333333333333</v>
+        <v>2.6666666666666665</v>
       </c>
       <c r="N59" s="3">
         <f>SUM(N2:N57)</f>
-        <v>2.3333333333333335</v>
+        <v>2.666666666666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fin de journée 20/05/2019 bis
Mise à jour planning effectif
</commit_message>
<xml_diff>
--- a/TPI/docs/Analyse/BJ_Planification.xlsx
+++ b/TPI/docs/Analyse/BJ_Planification.xlsx
@@ -3813,7 +3813,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N59"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
@@ -6123,8 +6123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K48" sqref="K48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7191,13 +7191,15 @@
       <c r="G43" s="4"/>
       <c r="H43" s="13"/>
       <c r="I43" s="4"/>
-      <c r="J43" s="13"/>
+      <c r="J43" s="13">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="K43" s="13"/>
       <c r="L43" s="4"/>
       <c r="M43" s="15"/>
       <c r="N43" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
@@ -7214,13 +7216,15 @@
       <c r="G44" s="4"/>
       <c r="H44" s="13"/>
       <c r="I44" s="4"/>
-      <c r="J44" s="13"/>
+      <c r="J44" s="13">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="K44" s="13"/>
       <c r="L44" s="4"/>
       <c r="M44" s="15"/>
       <c r="N44" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
@@ -7237,13 +7241,15 @@
       <c r="G45" s="4"/>
       <c r="H45" s="13"/>
       <c r="I45" s="4"/>
-      <c r="J45" s="13"/>
+      <c r="J45" s="13">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="K45" s="13"/>
       <c r="L45" s="4"/>
       <c r="M45" s="15"/>
       <c r="N45" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
@@ -7426,13 +7432,15 @@
       <c r="I53" s="4">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="J53" s="4"/>
+      <c r="J53" s="4">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="K53" s="4"/>
       <c r="L53" s="4"/>
       <c r="M53" s="15"/>
       <c r="N53" s="3">
         <f t="shared" ref="N53:N54" si="2">SUM(C53:M53)</f>
-        <v>0.27083333333333331</v>
+        <v>0.35416666666666663</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
@@ -7503,7 +7511,9 @@
       <c r="I56" s="13">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="J56" s="13"/>
+      <c r="J56" s="13">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="K56" s="13"/>
       <c r="L56" s="13"/>
       <c r="M56" s="15">
@@ -7511,7 +7521,7 @@
       </c>
       <c r="N56" s="3">
         <f>SUM(C56:M56)</f>
-        <v>0.82291666666666663</v>
+        <v>0.90625</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
@@ -7575,7 +7585,7 @@
       </c>
       <c r="J58" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="K58" s="3">
         <f t="shared" si="3"/>
@@ -7594,11 +7604,11 @@
       <c r="A59" s="40"/>
       <c r="M59" s="3">
         <f>SUM(C58:M58)</f>
-        <v>2.6666666666666665</v>
+        <v>3</v>
       </c>
       <c r="N59" s="3">
         <f>SUM(N2:N57)</f>
-        <v>2.666666666666667</v>
+        <v>3.0000000000000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fin de journée 21/05/2019
Suite de développement de la page calendrier
Modification de mes fonctions permettant d'envoyer un mail avec Swift Mailer
Suite documentation et création du fichier txt README.
</commit_message>
<xml_diff>
--- a/TPI/docs/Analyse/BJ_Planification.xlsx
+++ b/TPI/docs/Analyse/BJ_Planification.xlsx
@@ -294,7 +294,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -304,6 +304,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -437,7 +443,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -548,6 +554,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6123,8 +6130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K48" sqref="K48"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P42" sqref="P42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6781,12 +6788,14 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
+      <c r="K26" s="4">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="L26" s="4"/>
       <c r="M26" s="15"/>
       <c r="N26" s="3">
         <f t="shared" si="0"/>
-        <v>4.1666666666666664E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
@@ -6950,12 +6959,14 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="J33" s="13"/>
-      <c r="K33" s="13"/>
+      <c r="K33" s="13">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="L33" s="1"/>
       <c r="M33" s="15"/>
       <c r="N33" s="3">
         <f t="shared" si="0"/>
-        <v>4.1666666666666664E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
@@ -7244,12 +7255,14 @@
       <c r="J45" s="13">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="K45" s="13"/>
+      <c r="K45" s="13">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="L45" s="4"/>
       <c r="M45" s="15"/>
       <c r="N45" s="3">
         <f t="shared" si="0"/>
-        <v>4.1666666666666664E-2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
@@ -7267,7 +7280,7 @@
       <c r="H46" s="13"/>
       <c r="I46" s="4"/>
       <c r="J46" s="13"/>
-      <c r="K46" s="13"/>
+      <c r="K46" s="58"/>
       <c r="L46" s="4"/>
       <c r="M46" s="15"/>
       <c r="N46" s="3">
@@ -7290,12 +7303,14 @@
       <c r="H47" s="13"/>
       <c r="I47" s="4"/>
       <c r="J47" s="13"/>
-      <c r="K47" s="13"/>
+      <c r="K47" s="13">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="L47" s="4"/>
       <c r="M47" s="15"/>
       <c r="N47" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
@@ -7435,12 +7450,14 @@
       <c r="J53" s="4">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="K53" s="4"/>
+      <c r="K53" s="4">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="L53" s="4"/>
       <c r="M53" s="15"/>
       <c r="N53" s="3">
         <f t="shared" ref="N53:N54" si="2">SUM(C53:M53)</f>
-        <v>0.35416666666666663</v>
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
@@ -7514,14 +7531,16 @@
       <c r="J56" s="13">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="K56" s="13"/>
+      <c r="K56" s="13">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="L56" s="13"/>
       <c r="M56" s="15">
         <v>0.25</v>
       </c>
       <c r="N56" s="3">
         <f>SUM(C56:M56)</f>
-        <v>0.90625</v>
+        <v>0.98958333333333337</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
@@ -7589,7 +7608,7 @@
       </c>
       <c r="K58" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="L58" s="3">
         <f t="shared" si="3"/>
@@ -7604,11 +7623,11 @@
       <c r="A59" s="40"/>
       <c r="M59" s="3">
         <f>SUM(C58:M58)</f>
-        <v>3</v>
+        <v>3.3333333333333335</v>
       </c>
       <c r="N59" s="3">
         <f>SUM(N2:N57)</f>
-        <v>3.0000000000000004</v>
+        <v>3.3333333333333339</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fin de journée 22/05/2019
Développement de la page de statistique du réparateur
Suite et fin du développement de la page calendrier pour le réparateur
Suite documentation
</commit_message>
<xml_diff>
--- a/TPI/docs/Analyse/BJ_Planification.xlsx
+++ b/TPI/docs/Analyse/BJ_Planification.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21601"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JO-PC\Documents\GitHub\TPI_Borel-Jaquet\TPI\docs\Analyse\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMINC306\Documents\GitHub\TPI_Borel-Jaquet\TPI\docs\Analyse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9E84365-EEB1-4B20-82B2-368612F535A6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="690" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="690" windowWidth="19440" windowHeight="15000" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Planning prévisionnel" sheetId="1" r:id="rId1"/>
     <sheet name="Planning effectif" sheetId="5" r:id="rId2"/>
     <sheet name="Exemple" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -262,7 +261,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[hh]:mm"/>
   </numFmts>
@@ -554,21 +553,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="377">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="375">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -638,6 +623,20 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -1922,20 +1921,6 @@
       <fill>
         <patternFill>
           <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3508,23 +3493,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -3560,23 +3528,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3752,10 +3703,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
@@ -5230,777 +5181,777 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:M2 E3:E5 G3:G5 I3:I5 L3:L5 C51 E51:I51 L51 C54:C55 E54:E55 G54:G55 L54:L55 C56:L56 C40:C46 E40:E46 G40:G46 I40:I46 L40:L46">
-    <cfRule type="cellIs" dxfId="376" priority="229" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="374" priority="229" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:M2 D4:M5 C51:M51 C54:M56 C40:M46">
-    <cfRule type="cellIs" dxfId="375" priority="228" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="373" priority="228" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D51 G51 J51:K51">
-    <cfRule type="cellIs" dxfId="374" priority="224" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="372" priority="224" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:M5 C51:M51 C54:M56 C40:M46">
-    <cfRule type="cellIs" dxfId="373" priority="221" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="372" priority="222" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="371" priority="223" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="371" priority="221" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="370" priority="222" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="369" priority="223" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2 N54:N56 N43:N46">
-    <cfRule type="cellIs" dxfId="370" priority="214" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="368" priority="214" operator="greaterThan">
       <formula>$B2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="369" priority="220" operator="equal">
+    <cfRule type="cellIs" dxfId="367" priority="220" operator="equal">
       <formula>$B2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B57">
-    <cfRule type="cellIs" dxfId="368" priority="216" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="366" priority="216" operator="greaterThan">
       <formula>3.66666666666667</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="367" priority="218" operator="equal">
+    <cfRule type="cellIs" dxfId="365" priority="218" operator="equal">
       <formula>3.66666666666667</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C57:M57">
-    <cfRule type="cellIs" dxfId="366" priority="215" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="364" priority="215" operator="greaterThan">
       <formula>0.333333333333333</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="365" priority="217" operator="equal">
+    <cfRule type="cellIs" dxfId="363" priority="217" operator="equal">
       <formula>0.333333333333333</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N51 N3:N5">
-    <cfRule type="cellIs" dxfId="364" priority="212" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="362" priority="212" operator="greaterThan">
       <formula>$B3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="363" priority="213" operator="equal">
+    <cfRule type="cellIs" dxfId="361" priority="213" operator="equal">
       <formula>$B3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18 E18:I18 L18">
-    <cfRule type="cellIs" dxfId="362" priority="124" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="360" priority="124" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18:M18">
-    <cfRule type="cellIs" dxfId="361" priority="123" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="359" priority="123" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17:M17">
-    <cfRule type="cellIs" dxfId="360" priority="127" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="359" priority="128" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="358" priority="129" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="358" priority="127" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="357" priority="128" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="356" priority="129" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N18">
-    <cfRule type="cellIs" dxfId="357" priority="125" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="355" priority="125" operator="greaterThan">
       <formula>$B18</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="356" priority="126" operator="equal">
+    <cfRule type="cellIs" dxfId="354" priority="126" operator="equal">
       <formula>$B18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11 E11 G11 I11 L11">
-    <cfRule type="cellIs" dxfId="355" priority="183" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="353" priority="183" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11:M11">
-    <cfRule type="cellIs" dxfId="354" priority="182" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="352" priority="182" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:C10 E6:E10 G6:G10 I6:I10 L6:L10">
-    <cfRule type="cellIs" dxfId="353" priority="190" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="351" priority="190" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:M10">
-    <cfRule type="cellIs" dxfId="352" priority="189" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="350" priority="189" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:M10">
-    <cfRule type="cellIs" dxfId="351" priority="186" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="350" priority="187" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="349" priority="188" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="349" priority="186" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="348" priority="187" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="347" priority="188" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N6:N10">
-    <cfRule type="cellIs" dxfId="348" priority="184" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="346" priority="184" operator="greaterThan">
       <formula>$B6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="347" priority="185" operator="equal">
+    <cfRule type="cellIs" dxfId="345" priority="185" operator="equal">
       <formula>$B6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L11 I11 G11 E11 C11">
-    <cfRule type="cellIs" dxfId="346" priority="181" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="344" priority="181" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11:M11">
-    <cfRule type="cellIs" dxfId="345" priority="180" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="343" priority="180" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11:M11">
-    <cfRule type="cellIs" dxfId="344" priority="177" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="343" priority="178" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="342" priority="179" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="342" priority="177" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="341" priority="178" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="340" priority="179" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N11">
-    <cfRule type="cellIs" dxfId="341" priority="175" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="339" priority="175" operator="greaterThan">
       <formula>$B11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="340" priority="176" operator="equal">
+    <cfRule type="cellIs" dxfId="338" priority="176" operator="equal">
       <formula>$B11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N12">
-    <cfRule type="cellIs" dxfId="339" priority="173" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="337" priority="173" operator="greaterThan">
       <formula>$B12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="338" priority="174" operator="equal">
+    <cfRule type="cellIs" dxfId="336" priority="174" operator="equal">
       <formula>$B12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12 E12:I12 L12">
-    <cfRule type="cellIs" dxfId="337" priority="172" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="335" priority="172" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12:M12">
-    <cfRule type="cellIs" dxfId="336" priority="171" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="334" priority="171" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12 G12 J12:K12">
-    <cfRule type="cellIs" dxfId="335" priority="170" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="333" priority="170" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12:M12">
-    <cfRule type="cellIs" dxfId="334" priority="167" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="333" priority="168" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="332" priority="169" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="332" priority="167" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="331" priority="168" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="330" priority="169" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N13">
-    <cfRule type="cellIs" dxfId="331" priority="165" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="329" priority="165" operator="greaterThan">
       <formula>$B13</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="330" priority="166" operator="equal">
+    <cfRule type="cellIs" dxfId="328" priority="166" operator="equal">
       <formula>$B13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13 E13:I13 L13">
-    <cfRule type="cellIs" dxfId="329" priority="164" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="327" priority="164" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13:M13">
-    <cfRule type="cellIs" dxfId="328" priority="163" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="326" priority="163" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13 G13 J13:K13">
-    <cfRule type="cellIs" dxfId="327" priority="162" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="325" priority="162" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13:M13">
-    <cfRule type="cellIs" dxfId="326" priority="159" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="325" priority="160" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="324" priority="161" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="324" priority="159" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="323" priority="160" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="322" priority="161" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N14">
-    <cfRule type="cellIs" dxfId="323" priority="157" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="321" priority="157" operator="greaterThan">
       <formula>$B14</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="322" priority="158" operator="equal">
+    <cfRule type="cellIs" dxfId="320" priority="158" operator="equal">
       <formula>$B14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14 E14:I14 L14">
-    <cfRule type="cellIs" dxfId="321" priority="156" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="319" priority="156" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:M14">
-    <cfRule type="cellIs" dxfId="320" priority="155" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="318" priority="155" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14 G14 J14:K14">
-    <cfRule type="cellIs" dxfId="319" priority="154" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="317" priority="154" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:M14">
-    <cfRule type="cellIs" dxfId="318" priority="151" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="317" priority="152" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="316" priority="153" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="316" priority="151" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="315" priority="152" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="314" priority="153" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N15">
-    <cfRule type="cellIs" dxfId="315" priority="149" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="313" priority="149" operator="greaterThan">
       <formula>$B15</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="314" priority="150" operator="equal">
+    <cfRule type="cellIs" dxfId="312" priority="150" operator="equal">
       <formula>$B15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15 E15:I15 L15">
-    <cfRule type="cellIs" dxfId="313" priority="148" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="311" priority="148" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:M15">
-    <cfRule type="cellIs" dxfId="312" priority="147" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="310" priority="147" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15 G15 J15:K15">
-    <cfRule type="cellIs" dxfId="311" priority="146" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="309" priority="146" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:M15">
-    <cfRule type="cellIs" dxfId="310" priority="143" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="309" priority="144" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="308" priority="145" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="308" priority="143" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="307" priority="144" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="306" priority="145" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16:M16">
-    <cfRule type="cellIs" dxfId="307" priority="135" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="306" priority="136" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="305" priority="137" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="305" priority="135" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="304" priority="136" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="303" priority="137" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N16">
-    <cfRule type="cellIs" dxfId="304" priority="141" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="302" priority="141" operator="greaterThan">
       <formula>$B16</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="303" priority="142" operator="equal">
+    <cfRule type="cellIs" dxfId="301" priority="142" operator="equal">
       <formula>$B16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16 E16:I16 L16">
-    <cfRule type="cellIs" dxfId="302" priority="140" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="300" priority="140" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16:M16">
-    <cfRule type="cellIs" dxfId="301" priority="139" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="299" priority="139" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16 G16 J16:K16">
-    <cfRule type="cellIs" dxfId="300" priority="138" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="298" priority="138" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N17">
-    <cfRule type="cellIs" dxfId="299" priority="133" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="297" priority="133" operator="greaterThan">
       <formula>$B17</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="298" priority="134" operator="equal">
+    <cfRule type="cellIs" dxfId="296" priority="134" operator="equal">
       <formula>$B17</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17 E17:I17 L17">
-    <cfRule type="cellIs" dxfId="297" priority="132" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="295" priority="132" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17:M17">
-    <cfRule type="cellIs" dxfId="296" priority="131" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="294" priority="131" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D17 G17 J17:K17">
-    <cfRule type="cellIs" dxfId="295" priority="130" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="293" priority="130" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18:M18">
-    <cfRule type="cellIs" dxfId="294" priority="119" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="293" priority="120" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="292" priority="121" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="292" priority="119" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="291" priority="120" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="290" priority="121" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18 G18 J18:K18">
-    <cfRule type="cellIs" dxfId="291" priority="122" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="289" priority="122" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19:M19">
-    <cfRule type="cellIs" dxfId="290" priority="111" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="289" priority="112" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="288" priority="113" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="288" priority="111" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="287" priority="112" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="286" priority="113" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N19">
-    <cfRule type="cellIs" dxfId="287" priority="117" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="285" priority="117" operator="greaterThan">
       <formula>$B19</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="286" priority="118" operator="equal">
+    <cfRule type="cellIs" dxfId="284" priority="118" operator="equal">
       <formula>$B19</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19 E19:I19 L19">
-    <cfRule type="cellIs" dxfId="285" priority="116" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="283" priority="116" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19:M19">
-    <cfRule type="cellIs" dxfId="284" priority="115" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="282" priority="115" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D19 G19 J19:K19">
-    <cfRule type="cellIs" dxfId="283" priority="114" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="281" priority="114" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20:M20">
-    <cfRule type="cellIs" dxfId="282" priority="103" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="281" priority="104" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="280" priority="105" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="280" priority="103" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="279" priority="104" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="278" priority="105" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N20">
-    <cfRule type="cellIs" dxfId="279" priority="109" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="277" priority="109" operator="greaterThan">
       <formula>$B20</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="278" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="276" priority="110" operator="equal">
       <formula>$B20</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20 E20:I20 L20">
-    <cfRule type="cellIs" dxfId="277" priority="108" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="275" priority="108" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20:M20">
-    <cfRule type="cellIs" dxfId="276" priority="107" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="274" priority="107" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D20 G20 J20:K20">
-    <cfRule type="cellIs" dxfId="275" priority="106" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="273" priority="106" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:M21">
-    <cfRule type="cellIs" dxfId="274" priority="95" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="273" priority="96" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="272" priority="97" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="272" priority="95" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="271" priority="96" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="270" priority="97" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N21">
-    <cfRule type="cellIs" dxfId="271" priority="101" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="269" priority="101" operator="greaterThan">
       <formula>$B21</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="270" priority="102" operator="equal">
+    <cfRule type="cellIs" dxfId="268" priority="102" operator="equal">
       <formula>$B21</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21 E21:I21 L21">
-    <cfRule type="cellIs" dxfId="269" priority="100" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="267" priority="100" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:M21">
-    <cfRule type="cellIs" dxfId="268" priority="99" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="266" priority="99" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D21 G21 J21:K21">
-    <cfRule type="cellIs" dxfId="267" priority="98" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="265" priority="98" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C25 E22:E25 G22:G25 I22:I25 L22:L25">
-    <cfRule type="cellIs" dxfId="266" priority="94" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="264" priority="94" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:M25">
-    <cfRule type="cellIs" dxfId="265" priority="93" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="263" priority="93" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:M25">
-    <cfRule type="cellIs" dxfId="264" priority="90" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="263" priority="91" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="262" priority="92" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="262" priority="90" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="261" priority="91" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="260" priority="92" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N22:N25">
-    <cfRule type="cellIs" dxfId="261" priority="88" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="259" priority="88" operator="greaterThan">
       <formula>$B22</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="260" priority="89" operator="equal">
+    <cfRule type="cellIs" dxfId="258" priority="89" operator="equal">
       <formula>$B22</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26 E26:I26 L26">
-    <cfRule type="cellIs" dxfId="259" priority="87" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="257" priority="87" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:M26">
-    <cfRule type="cellIs" dxfId="258" priority="86" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="256" priority="86" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D26 G26 J26:K26">
-    <cfRule type="cellIs" dxfId="257" priority="85" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="255" priority="85" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:M26">
-    <cfRule type="cellIs" dxfId="256" priority="82" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="255" priority="83" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="254" priority="84" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="254" priority="82" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="253" priority="83" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="252" priority="84" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N26">
-    <cfRule type="cellIs" dxfId="253" priority="80" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="251" priority="80" operator="greaterThan">
       <formula>$B26</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="252" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="250" priority="81" operator="equal">
       <formula>$B26</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27 E27:I27 L27">
-    <cfRule type="cellIs" dxfId="251" priority="79" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="249" priority="79" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27:M27">
-    <cfRule type="cellIs" dxfId="250" priority="78" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="248" priority="78" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27 G27 J27:K27">
-    <cfRule type="cellIs" dxfId="249" priority="77" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="247" priority="77" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27:M27">
-    <cfRule type="cellIs" dxfId="248" priority="74" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="247" priority="75" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="246" priority="76" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="246" priority="74" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="245" priority="75" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="244" priority="76" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N27">
-    <cfRule type="cellIs" dxfId="245" priority="72" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="243" priority="72" operator="greaterThan">
       <formula>$B27</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="244" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="242" priority="73" operator="equal">
       <formula>$B27</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:C39 E28:E39 G28:G39 I28:I39 L28:L39">
-    <cfRule type="cellIs" dxfId="243" priority="71" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="241" priority="71" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:M39 C28:M33">
-    <cfRule type="cellIs" dxfId="242" priority="70" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="240" priority="70" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:M39">
-    <cfRule type="cellIs" dxfId="241" priority="67" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="240" priority="68" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="239" priority="69" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="239" priority="67" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="238" priority="68" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="237" priority="69" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N39 N28:N30">
-    <cfRule type="cellIs" dxfId="238" priority="65" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="236" priority="65" operator="greaterThan">
       <formula>$B28</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="237" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="235" priority="66" operator="equal">
       <formula>$B28</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N31:N38">
-    <cfRule type="cellIs" dxfId="236" priority="63" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="234" priority="63" operator="greaterThan">
       <formula>$B31</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="235" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="233" priority="64" operator="equal">
       <formula>$B31</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N40:N42">
-    <cfRule type="cellIs" dxfId="234" priority="47" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="232" priority="47" operator="greaterThan">
       <formula>$B40</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="233" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="231" priority="48" operator="equal">
       <formula>$B40</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C50 E48:E50 G48:G50 I48:I50 L48:L50">
-    <cfRule type="cellIs" dxfId="232" priority="46" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="230" priority="46" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:M50">
-    <cfRule type="cellIs" dxfId="231" priority="45" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="229" priority="45" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:M50">
-    <cfRule type="cellIs" dxfId="230" priority="42" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="229" priority="43" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="228" priority="44" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="228" priority="42" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="227" priority="43" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="226" priority="44" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N48:N50">
-    <cfRule type="cellIs" dxfId="227" priority="40" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="225" priority="40" operator="greaterThan">
       <formula>$B48</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="226" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="224" priority="41" operator="equal">
       <formula>$B48</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47 E47:I47 L47">
-    <cfRule type="cellIs" dxfId="225" priority="39" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="223" priority="39" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47:M47">
-    <cfRule type="cellIs" dxfId="224" priority="38" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="222" priority="38" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47 G47 J47:K47">
-    <cfRule type="cellIs" dxfId="223" priority="37" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="221" priority="37" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47:M47">
-    <cfRule type="cellIs" dxfId="222" priority="34" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="221" priority="35" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="220" priority="36" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="220" priority="34" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="219" priority="35" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="218" priority="36" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N47">
-    <cfRule type="cellIs" dxfId="219" priority="32" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="217" priority="32" operator="greaterThan">
       <formula>$B47</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="218" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="216" priority="33" operator="equal">
       <formula>$B47</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I54:I55">
-    <cfRule type="cellIs" dxfId="217" priority="31" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="215" priority="31" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L54 I54 G54 E54 C54">
-    <cfRule type="cellIs" dxfId="216" priority="23" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="214" priority="23" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54:M54">
-    <cfRule type="cellIs" dxfId="215" priority="22" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="213" priority="22" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C53:M53">
-    <cfRule type="cellIs" dxfId="214" priority="6" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="213" priority="7" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="212" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="212" priority="6" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="211" priority="7" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="210" priority="8" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N52">
-    <cfRule type="cellIs" dxfId="211" priority="20" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="209" priority="20" operator="greaterThan">
       <formula>$B52</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="210" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="208" priority="21" operator="equal">
       <formula>$B52</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C52 E52:I52 L52">
-    <cfRule type="cellIs" dxfId="209" priority="19" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="207" priority="19" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C52:M52">
-    <cfRule type="cellIs" dxfId="208" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="206" priority="18" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D52 G52 J52:K52">
-    <cfRule type="cellIs" dxfId="207" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="205" priority="17" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C52:M52">
-    <cfRule type="cellIs" dxfId="206" priority="14" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="205" priority="15" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="204" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="204" priority="14" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="203" priority="15" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="202" priority="16" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N53">
-    <cfRule type="cellIs" dxfId="203" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="201" priority="12" operator="greaterThan">
       <formula>$B53</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="202" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="200" priority="13" operator="equal">
       <formula>$B53</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C53 E53:I53 L53">
-    <cfRule type="cellIs" dxfId="201" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="199" priority="11" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C53:M53">
-    <cfRule type="cellIs" dxfId="200" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="198" priority="10" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D53 G53 J53:K53">
-    <cfRule type="cellIs" dxfId="199" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="197" priority="9" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C5">
-    <cfRule type="cellIs" dxfId="198" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="196" priority="5" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2 C4:C5">
-    <cfRule type="cellIs" dxfId="197" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="195" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C5">
-    <cfRule type="cellIs" dxfId="196" priority="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="195" priority="2" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="194" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="194" priority="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="193" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="192" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6010,11 +5961,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N58"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M49" sqref="M49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7091,11 +7042,13 @@
       <c r="K43" s="13">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="L43" s="4"/>
+      <c r="L43" s="4">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="M43" s="15"/>
       <c r="N43" s="3">
         <f t="shared" si="0"/>
-        <v>0.125</v>
+        <v>0.20833333333333331</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
@@ -7212,11 +7165,13 @@
       <c r="I48" s="4"/>
       <c r="J48" s="13"/>
       <c r="K48" s="13"/>
-      <c r="L48" s="4"/>
+      <c r="L48" s="4">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="M48" s="15"/>
       <c r="N48" s="3">
         <f>SUM(C48:M48)</f>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
@@ -7235,11 +7190,13 @@
       <c r="I49" s="4"/>
       <c r="J49" s="13"/>
       <c r="K49" s="13"/>
-      <c r="L49" s="4"/>
+      <c r="L49" s="4">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="M49" s="15"/>
       <c r="N49" s="3">
         <f t="shared" ref="N49:N50" si="1">SUM(C49:M49)</f>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
@@ -7394,13 +7351,15 @@
       <c r="K55" s="13">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="L55" s="13"/>
+      <c r="L55" s="13">
+        <v>0.125</v>
+      </c>
       <c r="M55" s="15">
         <v>0.25</v>
       </c>
       <c r="N55" s="3">
         <f>SUM(C55:M55)</f>
-        <v>0.98958333333333337</v>
+        <v>1.1145833333333335</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
@@ -7435,7 +7394,7 @@
         <v>3.6666666666666665</v>
       </c>
       <c r="C57" s="3">
-        <f t="shared" ref="B57:M57" si="4">SUM(C2:C56)</f>
+        <f t="shared" ref="C57:M57" si="4">SUM(C2:C56)</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="D57" s="3">
@@ -7472,7 +7431,7 @@
       </c>
       <c r="L57" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="M57" s="3">
         <f t="shared" si="4"/>
@@ -7483,45 +7442,45 @@
       <c r="A58" s="40"/>
       <c r="M58" s="3">
         <f>SUM(C57:M57)</f>
-        <v>3.3333333333333335</v>
+        <v>3.666666666666667</v>
       </c>
       <c r="N58" s="3">
         <f>SUM(N2:N56)</f>
-        <v>3.3333333333333339</v>
+        <v>3.666666666666667</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:M2 E3:E5 G3:G5 I3:I5 L3:L5 C51 E51:I51 L51 C54:C55 E54:E55 G54:G55 L54:L55 C56:L56 C40:C46 E40:E46 G40:G46 I40:I46 L40:L46">
-    <cfRule type="cellIs" dxfId="193" priority="192" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="191" priority="192" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:M2 D4:M5 C51:M51 C54:M56 C40:M46">
-    <cfRule type="cellIs" dxfId="192" priority="191" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="190" priority="191" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D51 G51 J51:K51">
-    <cfRule type="cellIs" dxfId="191" priority="190" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="189" priority="190" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:M5 C51:M51 C54:M56 C40:M46">
-    <cfRule type="cellIs" dxfId="190" priority="187" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="189" priority="188" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="188" priority="189" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="188" priority="187" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="187" priority="188" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="186" priority="189" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2 N54:N56 N43:N46">
-    <cfRule type="cellIs" dxfId="187" priority="181" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="185" priority="181" operator="greaterThan">
       <formula>$B2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="186" priority="186" operator="equal">
+    <cfRule type="cellIs" dxfId="184" priority="186" operator="equal">
       <formula>$B2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8259,10 +8218,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B57">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="greaterThan">
       <formula>3.66666666666667</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
       <formula>3.66666666666667</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8272,7 +8231,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -9000,43 +8959,43 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:L2 F24 H24:I24 C3:C20 E3:E20 G3:G20 I3:I20 K3:K20 C22:C26 G22:G26 I22:I23 I25:I26 E22:E26 K22:K26">
-    <cfRule type="cellIs" dxfId="10" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:L2 C4:L11 C13:L20 C22:L26">
-    <cfRule type="cellIs" dxfId="9" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K21 I21 G21 E21 C21">
-    <cfRule type="cellIs" dxfId="8" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:L21">
-    <cfRule type="cellIs" dxfId="7" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D25 F25 H25 J25 L25">
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D24 G24 J24">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:L26">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>